<commit_message>
Updating Bera_2011 Tidy Table
</commit_message>
<xml_diff>
--- a/in-progress/Koerner_2005_Polymer/Koerner_2005_Polymer_Tidy_Table.xlsx
+++ b/in-progress/Koerner_2005_Polymer/Koerner_2005_Polymer_Tidy_Table.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miked\Documents\GitHub\nmcuration\in-progress\Koerner_2005_Polymer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/in-progress/Koerner_2005_Polymer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310B4717-19AB-4CEF-A92F-582BC81E9146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5B7AFB-FBE7-AB42-9587-A4F692DB76ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AA27EEF6-2707-3642-A9D6-F1434A24BCB7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{AA27EEF6-2707-3642-A9D6-F1434A24BCB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Curation" sheetId="1" r:id="rId1"/>
     <sheet name="Tidy Table" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1931,6 +1933,45 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1938,6 +1979,60 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1966,93 +2061,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2087,12 +2095,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2413,36 +2415,36 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="65" customWidth="1"/>
-    <col min="3" max="3" width="121.796875" customWidth="1"/>
-    <col min="5" max="5" width="29.69921875" customWidth="1"/>
-    <col min="6" max="6" width="25.296875" customWidth="1"/>
+    <col min="3" max="3" width="121.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
-    <col min="8" max="8" width="29.796875" customWidth="1"/>
-    <col min="9" max="9" width="28.19921875" customWidth="1"/>
-    <col min="10" max="10" width="27.19921875" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" customWidth="1"/>
+    <col min="10" max="10" width="27.1640625" customWidth="1"/>
     <col min="11" max="11" width="28.5" customWidth="1"/>
     <col min="12" max="12" width="27.5" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
-    <col min="14" max="14" width="28.296875" customWidth="1"/>
-    <col min="15" max="15" width="29.796875" customWidth="1"/>
-    <col min="16" max="16" width="27.796875" customWidth="1"/>
-    <col min="17" max="17" width="27.19921875" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" customWidth="1"/>
+    <col min="15" max="15" width="29.83203125" customWidth="1"/>
+    <col min="16" max="16" width="27.83203125" customWidth="1"/>
+    <col min="17" max="17" width="27.1640625" customWidth="1"/>
     <col min="18" max="18" width="28.5" customWidth="1"/>
     <col min="19" max="19" width="27.5" customWidth="1"/>
-    <col min="20" max="20" width="29.796875" customWidth="1"/>
+    <col min="20" max="20" width="29.83203125" customWidth="1"/>
     <col min="21" max="21" width="28" customWidth="1"/>
-    <col min="22" max="22" width="26.796875" customWidth="1"/>
-    <col min="23" max="23" width="28.19921875" customWidth="1"/>
-    <col min="24" max="24" width="25.69921875" customWidth="1"/>
-    <col min="25" max="25" width="24.69921875" customWidth="1"/>
+    <col min="22" max="22" width="26.83203125" customWidth="1"/>
+    <col min="23" max="23" width="28.1640625" customWidth="1"/>
+    <col min="24" max="24" width="25.6640625" customWidth="1"/>
+    <col min="25" max="25" width="24.6640625" customWidth="1"/>
     <col min="26" max="26" width="21" customWidth="1"/>
-    <col min="27" max="27" width="26.19921875" customWidth="1"/>
+    <col min="27" max="27" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="16.2" thickBot="1"/>
+    <row r="1" spans="2:26" ht="17" thickBot="1"/>
     <row r="2" spans="2:26">
       <c r="B2" s="5" t="s">
         <v>17</v>
@@ -2459,7 +2461,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="16.2" thickBot="1">
+    <row r="4" spans="2:26" ht="17" thickBot="1">
       <c r="B4" s="13" t="s">
         <v>47</v>
       </c>
@@ -2467,8 +2469,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="16.2" thickBot="1"/>
-    <row r="6" spans="2:26" ht="16.2" thickBot="1">
+    <row r="5" spans="2:26" ht="17" thickBot="1"/>
+    <row r="6" spans="2:26" ht="17" thickBot="1">
       <c r="B6" s="16" t="s">
         <v>0</v>
       </c>
@@ -2476,7 +2478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="16.2" thickBot="1">
+    <row r="7" spans="2:26" ht="17" thickBot="1">
       <c r="B7" s="20" t="s">
         <v>60</v>
       </c>
@@ -2484,8 +2486,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B8" s="127" t="s">
+    <row r="8" spans="2:26" ht="17" thickBot="1">
+      <c r="B8" s="130" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -2498,19 +2500,19 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B9" s="128"/>
+    <row r="9" spans="2:26" ht="17" thickBot="1">
+      <c r="B9" s="125"/>
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="122" t="s">
+      <c r="E9" s="145" t="s">
         <v>162</v>
       </c>
-      <c r="F9" s="130"/>
-      <c r="G9" s="123"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="147"/>
     </row>
     <row r="10" spans="2:26">
-      <c r="B10" s="128"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
@@ -2523,41 +2525,41 @@
       <c r="G10" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="J10" s="122" t="s">
+      <c r="J10" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="K10" s="123"/>
-      <c r="L10" s="122" t="s">
+      <c r="K10" s="147"/>
+      <c r="L10" s="145" t="s">
         <v>180</v>
       </c>
-      <c r="M10" s="123"/>
-      <c r="N10" s="122" t="s">
+      <c r="M10" s="147"/>
+      <c r="N10" s="145" t="s">
         <v>181</v>
       </c>
-      <c r="O10" s="123"/>
-      <c r="P10" s="122" t="s">
+      <c r="O10" s="147"/>
+      <c r="P10" s="145" t="s">
         <v>182</v>
       </c>
-      <c r="Q10" s="123"/>
-      <c r="R10" s="122" t="s">
+      <c r="Q10" s="147"/>
+      <c r="R10" s="145" t="s">
         <v>183</v>
       </c>
-      <c r="S10" s="123"/>
-      <c r="U10" s="118" t="s">
+      <c r="S10" s="147"/>
+      <c r="U10" s="153" t="s">
         <v>253</v>
       </c>
-      <c r="V10" s="119"/>
-      <c r="W10" s="118" t="s">
+      <c r="V10" s="154"/>
+      <c r="W10" s="153" t="s">
         <v>255</v>
       </c>
-      <c r="X10" s="120"/>
-      <c r="Y10" s="121" t="s">
+      <c r="X10" s="155"/>
+      <c r="Y10" s="156" t="s">
         <v>254</v>
       </c>
-      <c r="Z10" s="120"/>
-    </row>
-    <row r="11" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B11" s="128"/>
+      <c r="Z10" s="155"/>
+    </row>
+    <row r="11" spans="2:26" ht="17" thickBot="1">
+      <c r="B11" s="125"/>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
@@ -2614,7 +2616,7 @@
       </c>
     </row>
     <row r="12" spans="2:26">
-      <c r="B12" s="128"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2677,7 +2679,7 @@
       </c>
     </row>
     <row r="13" spans="2:26">
-      <c r="B13" s="128"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
@@ -2739,11 +2741,11 @@
         <v>15.594099</v>
       </c>
     </row>
-    <row r="14" spans="2:26" ht="16.05" customHeight="1">
-      <c r="B14" s="137" t="s">
+    <row r="14" spans="2:26" ht="16" customHeight="1">
+      <c r="B14" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="132" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -2804,9 +2806,9 @@
         <v>17.235134599999999</v>
       </c>
     </row>
-    <row r="15" spans="2:26" ht="16.05" customHeight="1">
-      <c r="B15" s="137"/>
-      <c r="C15" s="138"/>
+    <row r="15" spans="2:26" ht="16" customHeight="1">
+      <c r="B15" s="131"/>
+      <c r="C15" s="132"/>
       <c r="E15" s="12" t="s">
         <v>170</v>
       </c>
@@ -2866,8 +2868,8 @@
       </c>
     </row>
     <row r="16" spans="2:26">
-      <c r="B16" s="137"/>
-      <c r="C16" s="138"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="132"/>
       <c r="E16" s="12" t="s">
         <v>171</v>
       </c>
@@ -2927,8 +2929,8 @@
       </c>
     </row>
     <row r="17" spans="2:26">
-      <c r="B17" s="137"/>
-      <c r="C17" s="138"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="132"/>
       <c r="E17" s="12" t="s">
         <v>172</v>
       </c>
@@ -2988,10 +2990,10 @@
       </c>
     </row>
     <row r="18" spans="2:26">
-      <c r="B18" s="136" t="s">
+      <c r="B18" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="133" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="12" t="s">
@@ -3053,8 +3055,8 @@
       </c>
     </row>
     <row r="19" spans="2:26">
-      <c r="B19" s="136"/>
-      <c r="C19" s="125"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="133"/>
       <c r="E19" s="12" t="s">
         <v>174</v>
       </c>
@@ -3113,9 +3115,9 @@
         <v>27.234399400000001</v>
       </c>
     </row>
-    <row r="20" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B20" s="136"/>
-      <c r="C20" s="125"/>
+    <row r="20" spans="2:26" ht="17" thickBot="1">
+      <c r="B20" s="134"/>
+      <c r="C20" s="133"/>
       <c r="E20" s="12" t="s">
         <v>175</v>
       </c>
@@ -3174,7 +3176,7 @@
         <v>28.277905100000002</v>
       </c>
     </row>
-    <row r="21" spans="2:26" ht="16.2" thickBot="1">
+    <row r="21" spans="2:26" ht="17" thickBot="1">
       <c r="B21" s="20" t="s">
         <v>62</v>
       </c>
@@ -3240,10 +3242,10 @@
       </c>
     </row>
     <row r="22" spans="2:26">
-      <c r="B22" s="137" t="s">
+      <c r="B22" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="138" t="s">
+      <c r="C22" s="132" t="s">
         <v>14</v>
       </c>
       <c r="J22" s="12">
@@ -3295,9 +3297,9 @@
         <v>29.915945600000001</v>
       </c>
     </row>
-    <row r="23" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B23" s="137"/>
-      <c r="C23" s="138"/>
+    <row r="23" spans="2:26" ht="17" thickBot="1">
+      <c r="B23" s="131"/>
+      <c r="C23" s="132"/>
       <c r="J23" s="12">
         <v>1.35455762059425</v>
       </c>
@@ -3347,15 +3349,15 @@
         <v>30.0627073</v>
       </c>
     </row>
-    <row r="24" spans="2:26" ht="16.05" customHeight="1" thickBot="1">
-      <c r="B24" s="137"/>
-      <c r="C24" s="138"/>
-      <c r="E24" s="110" t="s">
+    <row r="24" spans="2:26" ht="16" customHeight="1" thickBot="1">
+      <c r="B24" s="131"/>
+      <c r="C24" s="132"/>
+      <c r="E24" s="127" t="s">
         <v>184</v>
       </c>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="112"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="129"/>
       <c r="J24" s="12">
         <v>1.39607392036569</v>
       </c>
@@ -3405,9 +3407,9 @@
         <v>31.4021325</v>
       </c>
     </row>
-    <row r="25" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B25" s="137"/>
-      <c r="C25" s="138"/>
+    <row r="25" spans="2:26" ht="17" thickBot="1">
+      <c r="B25" s="131"/>
+      <c r="C25" s="132"/>
       <c r="E25" s="41" t="s">
         <v>163</v>
       </c>
@@ -3470,10 +3472,10 @@
       </c>
     </row>
     <row r="26" spans="2:26">
-      <c r="B26" s="128" t="s">
+      <c r="B26" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="125" t="s">
+      <c r="C26" s="133" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="32" t="s">
@@ -3538,8 +3540,8 @@
       </c>
     </row>
     <row r="27" spans="2:26">
-      <c r="B27" s="128"/>
-      <c r="C27" s="125"/>
+      <c r="B27" s="125"/>
+      <c r="C27" s="133"/>
       <c r="E27" s="12" t="s">
         <v>189</v>
       </c>
@@ -3602,10 +3604,10 @@
       </c>
     </row>
     <row r="28" spans="2:26">
-      <c r="B28" s="137" t="s">
+      <c r="B28" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="139" t="s">
+      <c r="C28" s="135" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -3670,8 +3672,8 @@
       </c>
     </row>
     <row r="29" spans="2:26">
-      <c r="B29" s="137"/>
-      <c r="C29" s="140"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="136"/>
       <c r="E29" s="12" t="s">
         <v>191</v>
       </c>
@@ -3734,8 +3736,8 @@
       </c>
     </row>
     <row r="30" spans="2:26">
-      <c r="B30" s="137"/>
-      <c r="C30" s="140"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="136"/>
       <c r="E30" s="12" t="s">
         <v>192</v>
       </c>
@@ -3798,8 +3800,8 @@
       </c>
     </row>
     <row r="31" spans="2:26">
-      <c r="B31" s="137"/>
-      <c r="C31" s="141"/>
+      <c r="B31" s="131"/>
+      <c r="C31" s="137"/>
       <c r="E31" s="12" t="s">
         <v>193</v>
       </c>
@@ -3861,11 +3863,11 @@
         <v>42.536554299999999</v>
       </c>
     </row>
-    <row r="32" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B32" s="128" t="s">
+    <row r="32" spans="2:26" ht="17" thickBot="1">
+      <c r="B32" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="125" t="s">
+      <c r="C32" s="133" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="13" t="s">
@@ -3929,9 +3931,9 @@
         <v>44.019746099999999</v>
       </c>
     </row>
-    <row r="33" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B33" s="128"/>
-      <c r="C33" s="125"/>
+    <row r="33" spans="2:26" ht="17" thickBot="1">
+      <c r="B33" s="125"/>
+      <c r="C33" s="133"/>
       <c r="J33" s="12">
         <v>1.76972061830867</v>
       </c>
@@ -3981,15 +3983,15 @@
         <v>43.709449900000003</v>
       </c>
     </row>
-    <row r="34" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B34" s="128"/>
-      <c r="C34" s="125"/>
-      <c r="E34" s="110" t="s">
+    <row r="34" spans="2:26" ht="17" thickBot="1">
+      <c r="B34" s="125"/>
+      <c r="C34" s="133"/>
+      <c r="E34" s="127" t="s">
         <v>195</v>
       </c>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="112"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="129"/>
       <c r="J34" s="12">
         <v>1.81123691808011</v>
       </c>
@@ -4021,11 +4023,11 @@
         <v>2.7804914799999998</v>
       </c>
     </row>
-    <row r="35" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B35" s="137" t="s">
+    <row r="35" spans="2:26" ht="17" thickBot="1">
+      <c r="B35" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="138" t="s">
+      <c r="C35" s="132" t="s">
         <v>25</v>
       </c>
       <c r="E35" s="41" t="s">
@@ -4072,8 +4074,8 @@
       </c>
     </row>
     <row r="36" spans="2:26">
-      <c r="B36" s="137"/>
-      <c r="C36" s="138"/>
+      <c r="B36" s="131"/>
+      <c r="C36" s="132"/>
       <c r="E36" s="32" t="s">
         <v>197</v>
       </c>
@@ -4118,8 +4120,8 @@
       </c>
     </row>
     <row r="37" spans="2:26">
-      <c r="B37" s="137"/>
-      <c r="C37" s="138"/>
+      <c r="B37" s="131"/>
+      <c r="C37" s="132"/>
       <c r="E37" s="12" t="s">
         <v>198</v>
       </c>
@@ -4163,11 +4165,11 @@
         <v>2.8744146100000001</v>
       </c>
     </row>
-    <row r="38" spans="2:26" ht="16.05" customHeight="1">
-      <c r="B38" s="128" t="s">
+    <row r="38" spans="2:26" ht="16" customHeight="1">
+      <c r="B38" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="125" t="s">
+      <c r="C38" s="133" t="s">
         <v>27</v>
       </c>
       <c r="E38" s="12" t="s">
@@ -4214,8 +4216,8 @@
       </c>
     </row>
     <row r="39" spans="2:26">
-      <c r="B39" s="128"/>
-      <c r="C39" s="125"/>
+      <c r="B39" s="125"/>
+      <c r="C39" s="133"/>
       <c r="E39" s="12" t="s">
         <v>200</v>
       </c>
@@ -4260,8 +4262,8 @@
       </c>
     </row>
     <row r="40" spans="2:26">
-      <c r="B40" s="128"/>
-      <c r="C40" s="125"/>
+      <c r="B40" s="125"/>
+      <c r="C40" s="133"/>
       <c r="E40" s="12" t="s">
         <v>201</v>
       </c>
@@ -4310,8 +4312,8 @@
       <c r="X40" s="27"/>
     </row>
     <row r="41" spans="2:26">
-      <c r="B41" s="128"/>
-      <c r="C41" s="125"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="133"/>
       <c r="E41" s="12" t="s">
         <v>202</v>
       </c>
@@ -4359,9 +4361,9 @@
       <c r="W41" s="27"/>
       <c r="X41" s="27"/>
     </row>
-    <row r="42" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B42" s="128"/>
-      <c r="C42" s="125"/>
+    <row r="42" spans="2:26" ht="17" thickBot="1">
+      <c r="B42" s="125"/>
+      <c r="C42" s="133"/>
       <c r="E42" s="13" t="s">
         <v>203</v>
       </c>
@@ -4409,9 +4411,9 @@
       <c r="W42" s="27"/>
       <c r="X42" s="27"/>
     </row>
-    <row r="43" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B43" s="128"/>
-      <c r="C43" s="125"/>
+    <row r="43" spans="2:26" ht="17" thickBot="1">
+      <c r="B43" s="125"/>
+      <c r="C43" s="133"/>
       <c r="E43" s="41" t="s">
         <v>163</v>
       </c>
@@ -4460,10 +4462,10 @@
       <c r="X43" s="27"/>
     </row>
     <row r="44" spans="2:26">
-      <c r="B44" s="137" t="s">
+      <c r="B44" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="138" t="s">
+      <c r="C44" s="132" t="s">
         <v>29</v>
       </c>
       <c r="E44" s="36" t="s">
@@ -4513,9 +4515,9 @@
       <c r="W44" s="27"/>
       <c r="X44" s="27"/>
     </row>
-    <row r="45" spans="2:26" ht="16.05" customHeight="1">
-      <c r="B45" s="137"/>
-      <c r="C45" s="138"/>
+    <row r="45" spans="2:26" ht="16" customHeight="1">
+      <c r="B45" s="131"/>
+      <c r="C45" s="132"/>
       <c r="E45" s="38" t="s">
         <v>205</v>
       </c>
@@ -4564,8 +4566,8 @@
       <c r="X45" s="27"/>
     </row>
     <row r="46" spans="2:26">
-      <c r="B46" s="137"/>
-      <c r="C46" s="138"/>
+      <c r="B46" s="131"/>
+      <c r="C46" s="132"/>
       <c r="E46" s="38" t="s">
         <v>206</v>
       </c>
@@ -4613,9 +4615,9 @@
       <c r="W46" s="27"/>
       <c r="X46" s="27"/>
     </row>
-    <row r="47" spans="2:26" ht="16.2" thickBot="1">
-      <c r="B47" s="137"/>
-      <c r="C47" s="138"/>
+    <row r="47" spans="2:26" ht="17" thickBot="1">
+      <c r="B47" s="131"/>
+      <c r="C47" s="132"/>
       <c r="E47" s="38" t="s">
         <v>207</v>
       </c>
@@ -4664,8 +4666,8 @@
       <c r="X47" s="27"/>
     </row>
     <row r="48" spans="2:26">
-      <c r="B48" s="137"/>
-      <c r="C48" s="138"/>
+      <c r="B48" s="131"/>
+      <c r="C48" s="132"/>
       <c r="E48" s="38" t="s">
         <v>208</v>
       </c>
@@ -4684,8 +4686,8 @@
       <c r="X48" s="27"/>
     </row>
     <row r="49" spans="2:24">
-      <c r="B49" s="137"/>
-      <c r="C49" s="138"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="132"/>
       <c r="E49" s="38" t="s">
         <v>209</v>
       </c>
@@ -4703,9 +4705,9 @@
       <c r="W49" s="27"/>
       <c r="X49" s="27"/>
     </row>
-    <row r="50" spans="2:24" ht="16.2" thickBot="1">
-      <c r="B50" s="137"/>
-      <c r="C50" s="138"/>
+    <row r="50" spans="2:24" ht="17" thickBot="1">
+      <c r="B50" s="131"/>
+      <c r="C50" s="132"/>
       <c r="E50" s="39" t="s">
         <v>210</v>
       </c>
@@ -4723,35 +4725,35 @@
       <c r="W50" s="27"/>
       <c r="X50" s="27"/>
     </row>
-    <row r="51" spans="2:24" ht="16.2" thickBot="1">
-      <c r="B51" s="137"/>
-      <c r="C51" s="138"/>
+    <row r="51" spans="2:24" ht="17" thickBot="1">
+      <c r="B51" s="131"/>
+      <c r="C51" s="132"/>
       <c r="U51" s="27"/>
       <c r="V51" s="27"/>
       <c r="W51" s="27"/>
       <c r="X51" s="27"/>
     </row>
-    <row r="52" spans="2:24" ht="16.2" thickBot="1">
-      <c r="B52" s="128" t="s">
+    <row r="52" spans="2:24" ht="17" thickBot="1">
+      <c r="B52" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="C52" s="125" t="s">
+      <c r="C52" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="E52" s="110" t="s">
+      <c r="E52" s="127" t="s">
         <v>212</v>
       </c>
-      <c r="F52" s="111"/>
-      <c r="G52" s="111"/>
-      <c r="H52" s="112"/>
+      <c r="F52" s="128"/>
+      <c r="G52" s="128"/>
+      <c r="H52" s="129"/>
       <c r="U52" s="27"/>
       <c r="V52" s="27"/>
       <c r="W52" s="27"/>
       <c r="X52" s="27"/>
     </row>
-    <row r="53" spans="2:24" ht="16.2" thickBot="1">
-      <c r="B53" s="128"/>
-      <c r="C53" s="125"/>
+    <row r="53" spans="2:24" ht="17" thickBot="1">
+      <c r="B53" s="125"/>
+      <c r="C53" s="133"/>
       <c r="E53" s="41" t="s">
         <v>163</v>
       </c>
@@ -4770,8 +4772,8 @@
       <c r="X53" s="27"/>
     </row>
     <row r="54" spans="2:24">
-      <c r="B54" s="128"/>
-      <c r="C54" s="125"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="133"/>
       <c r="E54" s="32" t="s">
         <v>213</v>
       </c>
@@ -4790,8 +4792,8 @@
       <c r="X54" s="27"/>
     </row>
     <row r="55" spans="2:24">
-      <c r="B55" s="128"/>
-      <c r="C55" s="125"/>
+      <c r="B55" s="125"/>
+      <c r="C55" s="133"/>
       <c r="E55" s="12" t="s">
         <v>214</v>
       </c>
@@ -4810,8 +4812,8 @@
       <c r="X55" s="27"/>
     </row>
     <row r="56" spans="2:24">
-      <c r="B56" s="128"/>
-      <c r="C56" s="125"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="133"/>
       <c r="E56" s="12" t="s">
         <v>215</v>
       </c>
@@ -4830,8 +4832,8 @@
       <c r="X56" s="27"/>
     </row>
     <row r="57" spans="2:24">
-      <c r="B57" s="128"/>
-      <c r="C57" s="125"/>
+      <c r="B57" s="125"/>
+      <c r="C57" s="133"/>
       <c r="E57" s="12" t="s">
         <v>216</v>
       </c>
@@ -4850,8 +4852,8 @@
       <c r="X57" s="27"/>
     </row>
     <row r="58" spans="2:24">
-      <c r="B58" s="128"/>
-      <c r="C58" s="125"/>
+      <c r="B58" s="125"/>
+      <c r="C58" s="133"/>
       <c r="E58" s="12" t="s">
         <v>217</v>
       </c>
@@ -4869,11 +4871,11 @@
       <c r="W58" s="27"/>
       <c r="X58" s="27"/>
     </row>
-    <row r="59" spans="2:24" ht="16.05" customHeight="1" thickBot="1">
-      <c r="B59" s="137" t="s">
+    <row r="59" spans="2:24" ht="16" customHeight="1" thickBot="1">
+      <c r="B59" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="C59" s="138" t="s">
+      <c r="C59" s="132" t="s">
         <v>34</v>
       </c>
       <c r="E59" s="34" t="s">
@@ -4893,9 +4895,9 @@
       <c r="W59" s="27"/>
       <c r="X59" s="27"/>
     </row>
-    <row r="60" spans="2:24" ht="16.2" thickBot="1">
-      <c r="B60" s="137"/>
-      <c r="C60" s="138"/>
+    <row r="60" spans="2:24" ht="17" thickBot="1">
+      <c r="B60" s="131"/>
+      <c r="C60" s="132"/>
       <c r="E60" s="41" t="s">
         <v>163</v>
       </c>
@@ -4914,8 +4916,8 @@
       <c r="X60" s="27"/>
     </row>
     <row r="61" spans="2:24">
-      <c r="B61" s="137"/>
-      <c r="C61" s="138"/>
+      <c r="B61" s="131"/>
+      <c r="C61" s="132"/>
       <c r="E61" s="44" t="s">
         <v>219</v>
       </c>
@@ -4934,8 +4936,8 @@
       <c r="X61" s="27"/>
     </row>
     <row r="62" spans="2:24">
-      <c r="B62" s="137"/>
-      <c r="C62" s="138"/>
+      <c r="B62" s="131"/>
+      <c r="C62" s="132"/>
       <c r="E62" s="38" t="s">
         <v>220</v>
       </c>
@@ -4954,8 +4956,8 @@
       <c r="X62" s="27"/>
     </row>
     <row r="63" spans="2:24">
-      <c r="B63" s="137"/>
-      <c r="C63" s="138"/>
+      <c r="B63" s="131"/>
+      <c r="C63" s="132"/>
       <c r="E63" s="38" t="s">
         <v>221</v>
       </c>
@@ -4973,7 +4975,7 @@
       <c r="W63" s="27"/>
       <c r="X63" s="27"/>
     </row>
-    <row r="64" spans="2:24">
+    <row r="64" spans="2:24" ht="17">
       <c r="B64" s="7" t="s">
         <v>36</v>
       </c>
@@ -4998,10 +5000,10 @@
       <c r="X64" s="27"/>
     </row>
     <row r="65" spans="2:8">
-      <c r="B65" s="128" t="s">
+      <c r="B65" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="125" t="s">
+      <c r="C65" s="133" t="s">
         <v>37</v>
       </c>
       <c r="E65" s="38" t="s">
@@ -5017,9 +5019,9 @@
         <v>2.2318772748788098</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B66" s="128"/>
-      <c r="C66" s="125"/>
+    <row r="66" spans="2:8" ht="17" thickBot="1">
+      <c r="B66" s="125"/>
+      <c r="C66" s="133"/>
       <c r="E66" s="39" t="s">
         <v>224</v>
       </c>
@@ -5033,7 +5035,7 @@
         <v>2.2206346809865001</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="16.2" thickBot="1">
+    <row r="67" spans="2:8" ht="17" thickBot="1">
       <c r="B67" s="9" t="s">
         <v>26</v>
       </c>
@@ -5045,23 +5047,23 @@
       <c r="G67" s="26"/>
       <c r="H67" s="26"/>
     </row>
-    <row r="68" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B68" s="128" t="s">
+    <row r="68" spans="2:8" ht="17" thickBot="1">
+      <c r="B68" s="125" t="s">
         <v>40</v>
       </c>
-      <c r="C68" s="125" t="s">
+      <c r="C68" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="E68" s="110" t="s">
+      <c r="E68" s="127" t="s">
         <v>239</v>
       </c>
-      <c r="F68" s="111"/>
-      <c r="G68" s="111"/>
-      <c r="H68" s="112"/>
-    </row>
-    <row r="69" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B69" s="128"/>
-      <c r="C69" s="125"/>
+      <c r="F68" s="128"/>
+      <c r="G68" s="128"/>
+      <c r="H68" s="129"/>
+    </row>
+    <row r="69" spans="2:8" ht="17" thickBot="1">
+      <c r="B69" s="125"/>
+      <c r="C69" s="133"/>
       <c r="E69" s="41" t="s">
         <v>163</v>
       </c>
@@ -5076,8 +5078,8 @@
       </c>
     </row>
     <row r="70" spans="2:8">
-      <c r="B70" s="128"/>
-      <c r="C70" s="125"/>
+      <c r="B70" s="125"/>
+      <c r="C70" s="133"/>
       <c r="E70" s="32" t="s">
         <v>228</v>
       </c>
@@ -5092,8 +5094,8 @@
       </c>
     </row>
     <row r="71" spans="2:8">
-      <c r="B71" s="128"/>
-      <c r="C71" s="125"/>
+      <c r="B71" s="125"/>
+      <c r="C71" s="133"/>
       <c r="E71" s="12" t="s">
         <v>229</v>
       </c>
@@ -5108,8 +5110,8 @@
       </c>
     </row>
     <row r="72" spans="2:8">
-      <c r="B72" s="128"/>
-      <c r="C72" s="125"/>
+      <c r="B72" s="125"/>
+      <c r="C72" s="133"/>
       <c r="E72" s="12" t="s">
         <v>230</v>
       </c>
@@ -5124,7 +5126,7 @@
       </c>
     </row>
     <row r="73" spans="2:8">
-      <c r="B73" s="128" t="s">
+      <c r="B73" s="125" t="s">
         <v>26</v>
       </c>
       <c r="C73" s="11" t="s">
@@ -5143,8 +5145,8 @@
         <v>31.190476190476101</v>
       </c>
     </row>
-    <row r="74" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B74" s="128"/>
+    <row r="74" spans="2:8" ht="17" thickBot="1">
+      <c r="B74" s="125"/>
       <c r="C74" s="11" t="s">
         <v>42</v>
       </c>
@@ -5161,9 +5163,9 @@
         <v>28.214285714285701</v>
       </c>
     </row>
-    <row r="75" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B75" s="128"/>
-      <c r="C75" s="125" t="s">
+    <row r="75" spans="2:8" ht="17" thickBot="1">
+      <c r="B75" s="125"/>
+      <c r="C75" s="133" t="s">
         <v>44</v>
       </c>
       <c r="E75" s="41" t="s">
@@ -5180,8 +5182,8 @@
       </c>
     </row>
     <row r="76" spans="2:8">
-      <c r="B76" s="128"/>
-      <c r="C76" s="125"/>
+      <c r="B76" s="125"/>
+      <c r="C76" s="133"/>
       <c r="E76" s="44" t="s">
         <v>233</v>
       </c>
@@ -5196,8 +5198,8 @@
       </c>
     </row>
     <row r="77" spans="2:8">
-      <c r="B77" s="128"/>
-      <c r="C77" s="125"/>
+      <c r="B77" s="125"/>
+      <c r="C77" s="133"/>
       <c r="E77" s="38" t="s">
         <v>234</v>
       </c>
@@ -5212,10 +5214,10 @@
       </c>
     </row>
     <row r="78" spans="2:8">
-      <c r="B78" s="128" t="s">
+      <c r="B78" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="C78" s="125" t="s">
+      <c r="C78" s="133" t="s">
         <v>45</v>
       </c>
       <c r="E78" s="38" t="s">
@@ -5231,9 +5233,9 @@
         <v>13.194259746472101</v>
       </c>
     </row>
-    <row r="79" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B79" s="128"/>
-      <c r="C79" s="125"/>
+    <row r="79" spans="2:8" ht="17" thickBot="1">
+      <c r="B79" s="125"/>
+      <c r="C79" s="133"/>
       <c r="E79" s="39" t="s">
         <v>236</v>
       </c>
@@ -5248,32 +5250,32 @@
       </c>
     </row>
     <row r="80" spans="2:8">
-      <c r="B80" s="128"/>
-      <c r="C80" s="125"/>
-    </row>
-    <row r="81" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B81" s="128"/>
-      <c r="C81" s="125"/>
+      <c r="B80" s="125"/>
+      <c r="C80" s="133"/>
+    </row>
+    <row r="81" spans="2:8" ht="17" thickBot="1">
+      <c r="B81" s="125"/>
+      <c r="C81" s="133"/>
       <c r="E81" s="27"/>
       <c r="F81" s="26"/>
       <c r="G81" s="26"/>
       <c r="H81" s="26"/>
     </row>
-    <row r="82" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B82" s="128"/>
-      <c r="C82" s="125"/>
-      <c r="E82" s="110" t="s">
+    <row r="82" spans="2:8" ht="17" thickBot="1">
+      <c r="B82" s="125"/>
+      <c r="C82" s="133"/>
+      <c r="E82" s="127" t="s">
         <v>81</v>
       </c>
-      <c r="F82" s="111"/>
-      <c r="G82" s="111"/>
-      <c r="H82" s="112"/>
-    </row>
-    <row r="83" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B83" s="128" t="s">
+      <c r="F82" s="128"/>
+      <c r="G82" s="128"/>
+      <c r="H82" s="129"/>
+    </row>
+    <row r="83" spans="2:8" ht="17" thickBot="1">
+      <c r="B83" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="C83" s="125" t="s">
+      <c r="C83" s="133" t="s">
         <v>49</v>
       </c>
       <c r="E83" s="16" t="s">
@@ -5289,19 +5291,19 @@
         <v>250</v>
       </c>
     </row>
-    <row r="84" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B84" s="128"/>
-      <c r="C84" s="125"/>
-      <c r="E84" s="113" t="s">
+    <row r="84" spans="2:8" ht="17" thickBot="1">
+      <c r="B84" s="125"/>
+      <c r="C84" s="133"/>
+      <c r="E84" s="148" t="s">
         <v>251</v>
       </c>
-      <c r="F84" s="114"/>
-      <c r="G84" s="114"/>
-      <c r="H84" s="115"/>
+      <c r="F84" s="149"/>
+      <c r="G84" s="149"/>
+      <c r="H84" s="150"/>
     </row>
     <row r="85" spans="2:8">
-      <c r="B85" s="128"/>
-      <c r="C85" s="125"/>
+      <c r="B85" s="125"/>
+      <c r="C85" s="133"/>
       <c r="E85" s="32" t="s">
         <v>240</v>
       </c>
@@ -5316,10 +5318,10 @@
       </c>
     </row>
     <row r="86" spans="2:8">
-      <c r="B86" s="128" t="s">
+      <c r="B86" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="C86" s="125" t="s">
+      <c r="C86" s="133" t="s">
         <v>52</v>
       </c>
       <c r="E86" s="12" t="s">
@@ -5336,8 +5338,8 @@
       </c>
     </row>
     <row r="87" spans="2:8">
-      <c r="B87" s="128"/>
-      <c r="C87" s="125"/>
+      <c r="B87" s="125"/>
+      <c r="C87" s="133"/>
       <c r="E87" s="12" t="s">
         <v>242</v>
       </c>
@@ -5352,8 +5354,8 @@
       </c>
     </row>
     <row r="88" spans="2:8">
-      <c r="B88" s="128"/>
-      <c r="C88" s="125"/>
+      <c r="B88" s="125"/>
+      <c r="C88" s="133"/>
       <c r="E88" s="12" t="s">
         <v>244</v>
       </c>
@@ -5367,11 +5369,11 @@
         <v>15.2380952380952</v>
       </c>
     </row>
-    <row r="89" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B89" s="128" t="s">
+    <row r="89" spans="2:8" ht="17" thickBot="1">
+      <c r="B89" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="C89" s="125" t="s">
+      <c r="C89" s="133" t="s">
         <v>53</v>
       </c>
       <c r="E89" s="12" t="s">
@@ -5387,19 +5389,19 @@
         <v>14.2312925170068</v>
       </c>
     </row>
-    <row r="90" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B90" s="128"/>
-      <c r="C90" s="125"/>
-      <c r="E90" s="113" t="s">
+    <row r="90" spans="2:8" ht="17" thickBot="1">
+      <c r="B90" s="125"/>
+      <c r="C90" s="133"/>
+      <c r="E90" s="148" t="s">
         <v>252</v>
       </c>
-      <c r="F90" s="116"/>
-      <c r="G90" s="116"/>
-      <c r="H90" s="117"/>
+      <c r="F90" s="151"/>
+      <c r="G90" s="151"/>
+      <c r="H90" s="152"/>
     </row>
     <row r="91" spans="2:8">
-      <c r="B91" s="128"/>
-      <c r="C91" s="125"/>
+      <c r="B91" s="125"/>
+      <c r="C91" s="133"/>
       <c r="E91" s="44" t="s">
         <v>245</v>
       </c>
@@ -5414,10 +5416,10 @@
       </c>
     </row>
     <row r="92" spans="2:8">
-      <c r="B92" s="128" t="s">
+      <c r="B92" s="125" t="s">
         <v>54</v>
       </c>
-      <c r="C92" s="125" t="s">
+      <c r="C92" s="133" t="s">
         <v>55</v>
       </c>
       <c r="E92" s="38" t="s">
@@ -5434,8 +5436,8 @@
       </c>
     </row>
     <row r="93" spans="2:8">
-      <c r="B93" s="128"/>
-      <c r="C93" s="125"/>
+      <c r="B93" s="125"/>
+      <c r="C93" s="133"/>
       <c r="E93" s="38" t="s">
         <v>247</v>
       </c>
@@ -5450,8 +5452,8 @@
       </c>
     </row>
     <row r="94" spans="2:8">
-      <c r="B94" s="128"/>
-      <c r="C94" s="125"/>
+      <c r="B94" s="125"/>
+      <c r="C94" s="133"/>
       <c r="E94" s="38" t="s">
         <v>248</v>
       </c>
@@ -5465,8 +5467,8 @@
         <v>4.8435374149659802</v>
       </c>
     </row>
-    <row r="95" spans="2:8" ht="16.2" thickBot="1">
-      <c r="B95" s="128" t="s">
+    <row r="95" spans="2:8" ht="17" thickBot="1">
+      <c r="B95" s="125" t="s">
         <v>26</v>
       </c>
       <c r="C95" s="10" t="s">
@@ -5486,16 +5488,16 @@
       </c>
     </row>
     <row r="96" spans="2:8">
-      <c r="B96" s="128"/>
-      <c r="C96" s="125" t="s">
+      <c r="B96" s="125"/>
+      <c r="C96" s="133" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="2:27" ht="16.2" thickBot="1">
-      <c r="B97" s="129"/>
-      <c r="C97" s="126"/>
-    </row>
-    <row r="98" spans="2:27" ht="16.2" thickBot="1">
+    <row r="97" spans="2:27" ht="17" thickBot="1">
+      <c r="B97" s="126"/>
+      <c r="C97" s="139"/>
+    </row>
+    <row r="98" spans="2:27" ht="17" thickBot="1">
       <c r="B98" s="18" t="s">
         <v>59</v>
       </c>
@@ -5504,53 +5506,53 @@
       </c>
     </row>
     <row r="99" spans="2:27">
-      <c r="B99" s="127" t="s">
+      <c r="B99" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="C99" s="124" t="s">
+      <c r="C99" s="138" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="100" spans="2:27" ht="16.2" thickBot="1">
-      <c r="B100" s="128"/>
-      <c r="C100" s="125"/>
-    </row>
-    <row r="101" spans="2:27" ht="16.2" thickBot="1">
-      <c r="B101" s="128" t="s">
+    <row r="100" spans="2:27" ht="17" thickBot="1">
+      <c r="B100" s="125"/>
+      <c r="C100" s="133"/>
+    </row>
+    <row r="101" spans="2:27" ht="17" thickBot="1">
+      <c r="B101" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="C101" s="125" t="s">
+      <c r="C101" s="133" t="s">
         <v>67</v>
       </c>
-      <c r="E101" s="110" t="s">
+      <c r="E101" s="127" t="s">
         <v>259</v>
       </c>
-      <c r="F101" s="111"/>
-      <c r="G101" s="111"/>
-      <c r="H101" s="111"/>
-      <c r="I101" s="111"/>
-      <c r="J101" s="111"/>
-      <c r="K101" s="111"/>
-      <c r="L101" s="111"/>
-      <c r="M101" s="111"/>
-      <c r="N101" s="111"/>
-      <c r="O101" s="111"/>
-      <c r="P101" s="111"/>
-      <c r="Q101" s="111"/>
-      <c r="R101" s="111"/>
-      <c r="S101" s="111"/>
-      <c r="T101" s="111"/>
-      <c r="U101" s="111"/>
-      <c r="V101" s="111"/>
-      <c r="W101" s="111"/>
-      <c r="X101" s="111"/>
-      <c r="Y101" s="111"/>
-      <c r="Z101" s="111"/>
-      <c r="AA101" s="112"/>
-    </row>
-    <row r="102" spans="2:27" ht="16.95" customHeight="1" thickBot="1">
-      <c r="B102" s="128"/>
-      <c r="C102" s="125"/>
+      <c r="F101" s="128"/>
+      <c r="G101" s="128"/>
+      <c r="H101" s="128"/>
+      <c r="I101" s="128"/>
+      <c r="J101" s="128"/>
+      <c r="K101" s="128"/>
+      <c r="L101" s="128"/>
+      <c r="M101" s="128"/>
+      <c r="N101" s="128"/>
+      <c r="O101" s="128"/>
+      <c r="P101" s="128"/>
+      <c r="Q101" s="128"/>
+      <c r="R101" s="128"/>
+      <c r="S101" s="128"/>
+      <c r="T101" s="128"/>
+      <c r="U101" s="128"/>
+      <c r="V101" s="128"/>
+      <c r="W101" s="128"/>
+      <c r="X101" s="128"/>
+      <c r="Y101" s="128"/>
+      <c r="Z101" s="128"/>
+      <c r="AA101" s="129"/>
+    </row>
+    <row r="102" spans="2:27" ht="17" customHeight="1" thickBot="1">
+      <c r="B102" s="125"/>
+      <c r="C102" s="133"/>
       <c r="E102" s="41" t="s">
         <v>268</v>
       </c>
@@ -5621,14 +5623,14 @@
         <v>270</v>
       </c>
     </row>
-    <row r="103" spans="2:27" ht="16.05" customHeight="1">
+    <row r="103" spans="2:27" ht="16" customHeight="1">
       <c r="B103" s="9" t="s">
         <v>68</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E103" s="142" t="s">
+      <c r="E103" s="116" t="s">
         <v>162</v>
       </c>
       <c r="F103" s="63" t="s">
@@ -5661,13 +5663,13 @@
       <c r="AA103" s="52"/>
     </row>
     <row r="104" spans="2:27">
-      <c r="B104" s="128" t="s">
+      <c r="B104" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="C104" s="125" t="s">
+      <c r="C104" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="E104" s="143"/>
+      <c r="E104" s="117"/>
       <c r="F104" s="60" t="s">
         <v>167</v>
       </c>
@@ -5698,9 +5700,9 @@
       <c r="AA104" s="53"/>
     </row>
     <row r="105" spans="2:27">
-      <c r="B105" s="128"/>
-      <c r="C105" s="125"/>
-      <c r="E105" s="143"/>
+      <c r="B105" s="125"/>
+      <c r="C105" s="133"/>
+      <c r="E105" s="117"/>
       <c r="F105" s="60" t="s">
         <v>168</v>
       </c>
@@ -5731,9 +5733,9 @@
       <c r="AA105" s="53"/>
     </row>
     <row r="106" spans="2:27">
-      <c r="B106" s="128"/>
-      <c r="C106" s="125"/>
-      <c r="E106" s="143"/>
+      <c r="B106" s="125"/>
+      <c r="C106" s="133"/>
+      <c r="E106" s="117"/>
       <c r="F106" s="60" t="s">
         <v>169</v>
       </c>
@@ -5764,13 +5766,13 @@
       <c r="AA106" s="53"/>
     </row>
     <row r="107" spans="2:27">
-      <c r="B107" s="128" t="s">
+      <c r="B107" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="C107" s="125" t="s">
+      <c r="C107" s="133" t="s">
         <v>72</v>
       </c>
-      <c r="E107" s="143"/>
+      <c r="E107" s="117"/>
       <c r="F107" s="60" t="s">
         <v>170</v>
       </c>
@@ -5801,9 +5803,9 @@
       <c r="AA107" s="53"/>
     </row>
     <row r="108" spans="2:27">
-      <c r="B108" s="128"/>
-      <c r="C108" s="125"/>
-      <c r="E108" s="143"/>
+      <c r="B108" s="125"/>
+      <c r="C108" s="133"/>
+      <c r="E108" s="117"/>
       <c r="F108" s="60" t="s">
         <v>171</v>
       </c>
@@ -5834,9 +5836,9 @@
       <c r="AA108" s="53"/>
     </row>
     <row r="109" spans="2:27">
-      <c r="B109" s="128"/>
-      <c r="C109" s="125"/>
-      <c r="E109" s="143"/>
+      <c r="B109" s="125"/>
+      <c r="C109" s="133"/>
+      <c r="E109" s="117"/>
       <c r="F109" s="60" t="s">
         <v>172</v>
       </c>
@@ -5867,9 +5869,9 @@
       <c r="AA109" s="53"/>
     </row>
     <row r="110" spans="2:27">
-      <c r="B110" s="128"/>
-      <c r="C110" s="125"/>
-      <c r="E110" s="143"/>
+      <c r="B110" s="125"/>
+      <c r="C110" s="133"/>
+      <c r="E110" s="117"/>
       <c r="F110" s="60" t="s">
         <v>173</v>
       </c>
@@ -5900,9 +5902,9 @@
       <c r="AA110" s="53"/>
     </row>
     <row r="111" spans="2:27">
-      <c r="B111" s="128"/>
-      <c r="C111" s="125"/>
-      <c r="E111" s="143"/>
+      <c r="B111" s="125"/>
+      <c r="C111" s="133"/>
+      <c r="E111" s="117"/>
       <c r="F111" s="60" t="s">
         <v>174</v>
       </c>
@@ -5933,9 +5935,9 @@
       <c r="AA111" s="53"/>
     </row>
     <row r="112" spans="2:27">
-      <c r="B112" s="128"/>
-      <c r="C112" s="125"/>
-      <c r="E112" s="143"/>
+      <c r="B112" s="125"/>
+      <c r="C112" s="133"/>
+      <c r="E112" s="117"/>
       <c r="F112" s="60" t="s">
         <v>175</v>
       </c>
@@ -5965,10 +5967,10 @@
       <c r="Z112" s="48"/>
       <c r="AA112" s="53"/>
     </row>
-    <row r="113" spans="2:27" ht="16.2" thickBot="1">
-      <c r="B113" s="128"/>
-      <c r="C113" s="125"/>
-      <c r="E113" s="144"/>
+    <row r="113" spans="2:27" ht="17" thickBot="1">
+      <c r="B113" s="125"/>
+      <c r="C113" s="133"/>
+      <c r="E113" s="118"/>
       <c r="F113" s="61" t="s">
         <v>176</v>
       </c>
@@ -5998,15 +6000,15 @@
       <c r="Z113" s="54"/>
       <c r="AA113" s="55"/>
     </row>
-    <row r="114" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B114" s="128" t="s">
+    <row r="114" spans="2:27" ht="16" customHeight="1">
+      <c r="B114" s="125" t="s">
         <v>106</v>
       </c>
-      <c r="C114" s="125"/>
-      <c r="E114" s="145" t="s">
+      <c r="C114" s="133"/>
+      <c r="E114" s="119" t="s">
         <v>261</v>
       </c>
-      <c r="F114" s="147" t="s">
+      <c r="F114" s="121" t="s">
         <v>262</v>
       </c>
       <c r="G114" s="50"/>
@@ -6050,10 +6052,10 @@
       <c r="AA114" s="62"/>
     </row>
     <row r="115" spans="2:27">
-      <c r="B115" s="128"/>
-      <c r="C115" s="125"/>
-      <c r="E115" s="143"/>
-      <c r="F115" s="148"/>
+      <c r="B115" s="125"/>
+      <c r="C115" s="133"/>
+      <c r="E115" s="117"/>
+      <c r="F115" s="122"/>
       <c r="G115" s="48"/>
       <c r="H115" s="48"/>
       <c r="I115" s="48"/>
@@ -6095,12 +6097,12 @@
       <c r="AA115" s="53"/>
     </row>
     <row r="116" spans="2:27">
-      <c r="B116" s="128" t="s">
+      <c r="B116" s="125" t="s">
         <v>108</v>
       </c>
-      <c r="C116" s="125"/>
-      <c r="E116" s="143"/>
-      <c r="F116" s="148"/>
+      <c r="C116" s="133"/>
+      <c r="E116" s="117"/>
+      <c r="F116" s="122"/>
       <c r="G116" s="48"/>
       <c r="H116" s="48"/>
       <c r="I116" s="48"/>
@@ -6142,10 +6144,10 @@
       <c r="AA116" s="53"/>
     </row>
     <row r="117" spans="2:27">
-      <c r="B117" s="128"/>
-      <c r="C117" s="125"/>
-      <c r="E117" s="143"/>
-      <c r="F117" s="148"/>
+      <c r="B117" s="125"/>
+      <c r="C117" s="133"/>
+      <c r="E117" s="117"/>
+      <c r="F117" s="122"/>
       <c r="G117" s="48"/>
       <c r="H117" s="48"/>
       <c r="I117" s="48"/>
@@ -6187,10 +6189,10 @@
       <c r="AA117" s="53"/>
     </row>
     <row r="118" spans="2:27">
-      <c r="B118" s="128"/>
-      <c r="C118" s="125"/>
-      <c r="E118" s="143"/>
-      <c r="F118" s="148"/>
+      <c r="B118" s="125"/>
+      <c r="C118" s="133"/>
+      <c r="E118" s="117"/>
+      <c r="F118" s="122"/>
       <c r="G118" s="48"/>
       <c r="H118" s="48"/>
       <c r="I118" s="48"/>
@@ -6232,10 +6234,10 @@
       <c r="AA118" s="53"/>
     </row>
     <row r="119" spans="2:27">
-      <c r="B119" s="128"/>
-      <c r="C119" s="125"/>
-      <c r="E119" s="143"/>
-      <c r="F119" s="148"/>
+      <c r="B119" s="125"/>
+      <c r="C119" s="133"/>
+      <c r="E119" s="117"/>
+      <c r="F119" s="122"/>
       <c r="G119" s="48"/>
       <c r="H119" s="48"/>
       <c r="I119" s="48"/>
@@ -6277,14 +6279,14 @@
       <c r="AA119" s="53"/>
     </row>
     <row r="120" spans="2:27">
-      <c r="B120" s="136" t="s">
+      <c r="B120" s="134" t="s">
         <v>26</v>
       </c>
       <c r="C120" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E120" s="143"/>
-      <c r="F120" s="148"/>
+      <c r="E120" s="117"/>
+      <c r="F120" s="122"/>
       <c r="G120" s="48"/>
       <c r="H120" s="48"/>
       <c r="I120" s="48"/>
@@ -6325,13 +6327,13 @@
       <c r="Z120" s="48"/>
       <c r="AA120" s="53"/>
     </row>
-    <row r="121" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B121" s="136"/>
-      <c r="C121" s="125" t="s">
+    <row r="121" spans="2:27" ht="16" customHeight="1">
+      <c r="B121" s="134"/>
+      <c r="C121" s="133" t="s">
         <v>75</v>
       </c>
-      <c r="E121" s="143"/>
-      <c r="F121" s="148"/>
+      <c r="E121" s="117"/>
+      <c r="F121" s="122"/>
       <c r="G121" s="48"/>
       <c r="H121" s="48"/>
       <c r="I121" s="48"/>
@@ -6372,11 +6374,11 @@
       <c r="Z121" s="48"/>
       <c r="AA121" s="53"/>
     </row>
-    <row r="122" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B122" s="136"/>
-      <c r="C122" s="125"/>
-      <c r="E122" s="143"/>
-      <c r="F122" s="148"/>
+    <row r="122" spans="2:27" ht="16" customHeight="1">
+      <c r="B122" s="134"/>
+      <c r="C122" s="133"/>
+      <c r="E122" s="117"/>
+      <c r="F122" s="122"/>
       <c r="G122" s="48"/>
       <c r="H122" s="48"/>
       <c r="I122" s="48"/>
@@ -6417,13 +6419,13 @@
       <c r="Z122" s="48"/>
       <c r="AA122" s="53"/>
     </row>
-    <row r="123" spans="2:27" ht="16.95" customHeight="1">
-      <c r="B123" s="136"/>
+    <row r="123" spans="2:27" ht="17" customHeight="1">
+      <c r="B123" s="134"/>
       <c r="C123" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E123" s="143"/>
-      <c r="F123" s="148"/>
+      <c r="E123" s="117"/>
+      <c r="F123" s="122"/>
       <c r="G123" s="48"/>
       <c r="H123" s="48"/>
       <c r="I123" s="48"/>
@@ -6464,15 +6466,15 @@
       <c r="Z123" s="48"/>
       <c r="AA123" s="53"/>
     </row>
-    <row r="124" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B124" s="128" t="s">
+    <row r="124" spans="2:27" ht="16" customHeight="1">
+      <c r="B124" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="C124" s="125" t="s">
+      <c r="C124" s="133" t="s">
         <v>78</v>
       </c>
-      <c r="E124" s="143"/>
-      <c r="F124" s="148"/>
+      <c r="E124" s="117"/>
+      <c r="F124" s="122"/>
       <c r="G124" s="48"/>
       <c r="H124" s="48"/>
       <c r="I124" s="48"/>
@@ -6514,10 +6516,10 @@
       <c r="AA124" s="53"/>
     </row>
     <row r="125" spans="2:27">
-      <c r="B125" s="128"/>
-      <c r="C125" s="125"/>
-      <c r="E125" s="143"/>
-      <c r="F125" s="148"/>
+      <c r="B125" s="125"/>
+      <c r="C125" s="133"/>
+      <c r="E125" s="117"/>
+      <c r="F125" s="122"/>
       <c r="G125" s="48"/>
       <c r="H125" s="48"/>
       <c r="I125" s="48"/>
@@ -6559,12 +6561,12 @@
       <c r="AA125" s="53"/>
     </row>
     <row r="126" spans="2:27">
-      <c r="B126" s="128"/>
-      <c r="C126" s="125" t="s">
+      <c r="B126" s="125"/>
+      <c r="C126" s="133" t="s">
         <v>79</v>
       </c>
-      <c r="E126" s="143"/>
-      <c r="F126" s="148"/>
+      <c r="E126" s="117"/>
+      <c r="F126" s="122"/>
       <c r="G126" s="48"/>
       <c r="H126" s="48"/>
       <c r="I126" s="48"/>
@@ -6606,10 +6608,10 @@
       <c r="AA126" s="53"/>
     </row>
     <row r="127" spans="2:27">
-      <c r="B127" s="128"/>
-      <c r="C127" s="125"/>
-      <c r="E127" s="143"/>
-      <c r="F127" s="148"/>
+      <c r="B127" s="125"/>
+      <c r="C127" s="133"/>
+      <c r="E127" s="117"/>
+      <c r="F127" s="122"/>
       <c r="G127" s="48"/>
       <c r="H127" s="48"/>
       <c r="I127" s="48"/>
@@ -6651,10 +6653,10 @@
       <c r="AA127" s="53"/>
     </row>
     <row r="128" spans="2:27">
-      <c r="B128" s="128"/>
-      <c r="C128" s="125"/>
-      <c r="E128" s="143"/>
-      <c r="F128" s="148"/>
+      <c r="B128" s="125"/>
+      <c r="C128" s="133"/>
+      <c r="E128" s="117"/>
+      <c r="F128" s="122"/>
       <c r="G128" s="48"/>
       <c r="H128" s="48"/>
       <c r="I128" s="48"/>
@@ -6695,15 +6697,15 @@
       <c r="Z128" s="48"/>
       <c r="AA128" s="53"/>
     </row>
-    <row r="129" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B129" s="128" t="s">
+    <row r="129" spans="2:27" ht="16" customHeight="1">
+      <c r="B129" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="C129" s="125" t="s">
+      <c r="C129" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="E129" s="143"/>
-      <c r="F129" s="148"/>
+      <c r="E129" s="117"/>
+      <c r="F129" s="122"/>
       <c r="G129" s="48"/>
       <c r="H129" s="48"/>
       <c r="I129" s="48"/>
@@ -6745,10 +6747,10 @@
       <c r="AA129" s="53"/>
     </row>
     <row r="130" spans="2:27">
-      <c r="B130" s="128"/>
-      <c r="C130" s="125"/>
-      <c r="E130" s="143"/>
-      <c r="F130" s="148"/>
+      <c r="B130" s="125"/>
+      <c r="C130" s="133"/>
+      <c r="E130" s="117"/>
+      <c r="F130" s="122"/>
       <c r="G130" s="48"/>
       <c r="H130" s="48"/>
       <c r="I130" s="48"/>
@@ -6790,12 +6792,12 @@
       <c r="AA130" s="53"/>
     </row>
     <row r="131" spans="2:27">
-      <c r="B131" s="128" t="s">
+      <c r="B131" s="125" t="s">
         <v>107</v>
       </c>
-      <c r="C131" s="125"/>
-      <c r="E131" s="143"/>
-      <c r="F131" s="148"/>
+      <c r="C131" s="133"/>
+      <c r="E131" s="117"/>
+      <c r="F131" s="122"/>
       <c r="G131" s="48"/>
       <c r="H131" s="48"/>
       <c r="I131" s="48"/>
@@ -6837,10 +6839,10 @@
       <c r="AA131" s="53"/>
     </row>
     <row r="132" spans="2:27">
-      <c r="B132" s="128"/>
-      <c r="C132" s="125"/>
-      <c r="E132" s="143"/>
-      <c r="F132" s="148"/>
+      <c r="B132" s="125"/>
+      <c r="C132" s="133"/>
+      <c r="E132" s="117"/>
+      <c r="F132" s="122"/>
       <c r="G132" s="48"/>
       <c r="H132" s="48"/>
       <c r="I132" s="48"/>
@@ -6882,14 +6884,14 @@
       <c r="AA132" s="53"/>
     </row>
     <row r="133" spans="2:27">
-      <c r="B133" s="128" t="s">
+      <c r="B133" s="125" t="s">
         <v>82</v>
       </c>
-      <c r="C133" s="125" t="s">
+      <c r="C133" s="133" t="s">
         <v>83</v>
       </c>
-      <c r="E133" s="143"/>
-      <c r="F133" s="148"/>
+      <c r="E133" s="117"/>
+      <c r="F133" s="122"/>
       <c r="G133" s="48"/>
       <c r="H133" s="48"/>
       <c r="I133" s="48"/>
@@ -6931,10 +6933,10 @@
       <c r="AA133" s="53"/>
     </row>
     <row r="134" spans="2:27">
-      <c r="B134" s="128"/>
-      <c r="C134" s="125"/>
-      <c r="E134" s="143"/>
-      <c r="F134" s="148"/>
+      <c r="B134" s="125"/>
+      <c r="C134" s="133"/>
+      <c r="E134" s="117"/>
+      <c r="F134" s="122"/>
       <c r="G134" s="48"/>
       <c r="H134" s="48"/>
       <c r="I134" s="48"/>
@@ -6976,10 +6978,10 @@
       <c r="AA134" s="53"/>
     </row>
     <row r="135" spans="2:27">
-      <c r="B135" s="128"/>
-      <c r="C135" s="125"/>
-      <c r="E135" s="143"/>
-      <c r="F135" s="148"/>
+      <c r="B135" s="125"/>
+      <c r="C135" s="133"/>
+      <c r="E135" s="117"/>
+      <c r="F135" s="122"/>
       <c r="G135" s="48"/>
       <c r="H135" s="48"/>
       <c r="I135" s="48"/>
@@ -7021,14 +7023,14 @@
       <c r="AA135" s="53"/>
     </row>
     <row r="136" spans="2:27">
-      <c r="B136" s="128" t="s">
+      <c r="B136" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="C136" s="132" t="s">
+      <c r="C136" s="141" t="s">
         <v>85</v>
       </c>
-      <c r="E136" s="143"/>
-      <c r="F136" s="148"/>
+      <c r="E136" s="117"/>
+      <c r="F136" s="122"/>
       <c r="G136" s="48"/>
       <c r="H136" s="48"/>
       <c r="I136" s="48"/>
@@ -7069,11 +7071,11 @@
       <c r="Z136" s="48"/>
       <c r="AA136" s="53"/>
     </row>
-    <row r="137" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B137" s="128"/>
-      <c r="C137" s="135"/>
-      <c r="E137" s="143"/>
-      <c r="F137" s="148"/>
+    <row r="137" spans="2:27" ht="16" customHeight="1">
+      <c r="B137" s="125"/>
+      <c r="C137" s="142"/>
+      <c r="E137" s="117"/>
+      <c r="F137" s="122"/>
       <c r="G137" s="48"/>
       <c r="H137" s="48"/>
       <c r="I137" s="48"/>
@@ -7115,10 +7117,10 @@
       <c r="AA137" s="53"/>
     </row>
     <row r="138" spans="2:27">
-      <c r="B138" s="128"/>
-      <c r="C138" s="135"/>
-      <c r="E138" s="143"/>
-      <c r="F138" s="148"/>
+      <c r="B138" s="125"/>
+      <c r="C138" s="142"/>
+      <c r="E138" s="117"/>
+      <c r="F138" s="122"/>
       <c r="G138" s="48"/>
       <c r="H138" s="48"/>
       <c r="I138" s="48"/>
@@ -7160,10 +7162,10 @@
       <c r="AA138" s="53"/>
     </row>
     <row r="139" spans="2:27">
-      <c r="B139" s="128"/>
-      <c r="C139" s="135"/>
-      <c r="E139" s="143"/>
-      <c r="F139" s="148"/>
+      <c r="B139" s="125"/>
+      <c r="C139" s="142"/>
+      <c r="E139" s="117"/>
+      <c r="F139" s="122"/>
       <c r="G139" s="48"/>
       <c r="H139" s="48"/>
       <c r="I139" s="48"/>
@@ -7205,10 +7207,10 @@
       <c r="AA139" s="53"/>
     </row>
     <row r="140" spans="2:27">
-      <c r="B140" s="128"/>
-      <c r="C140" s="124"/>
-      <c r="E140" s="143"/>
-      <c r="F140" s="148"/>
+      <c r="B140" s="125"/>
+      <c r="C140" s="138"/>
+      <c r="E140" s="117"/>
+      <c r="F140" s="122"/>
       <c r="G140" s="48"/>
       <c r="H140" s="48"/>
       <c r="I140" s="48"/>
@@ -7250,14 +7252,14 @@
       <c r="AA140" s="53"/>
     </row>
     <row r="141" spans="2:27">
-      <c r="B141" s="128" t="s">
+      <c r="B141" s="125" t="s">
         <v>86</v>
       </c>
-      <c r="C141" s="125" t="s">
+      <c r="C141" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="E141" s="143"/>
-      <c r="F141" s="148"/>
+      <c r="E141" s="117"/>
+      <c r="F141" s="122"/>
       <c r="G141" s="48"/>
       <c r="H141" s="48"/>
       <c r="I141" s="48"/>
@@ -7298,11 +7300,11 @@
       <c r="Z141" s="48"/>
       <c r="AA141" s="53"/>
     </row>
-    <row r="142" spans="2:27" ht="16.95" customHeight="1">
-      <c r="B142" s="128"/>
-      <c r="C142" s="125"/>
-      <c r="E142" s="143"/>
-      <c r="F142" s="148"/>
+    <row r="142" spans="2:27" ht="17" customHeight="1">
+      <c r="B142" s="125"/>
+      <c r="C142" s="133"/>
+      <c r="E142" s="117"/>
+      <c r="F142" s="122"/>
       <c r="G142" s="48"/>
       <c r="H142" s="48"/>
       <c r="I142" s="48"/>
@@ -7344,10 +7346,10 @@
       <c r="AA142" s="53"/>
     </row>
     <row r="143" spans="2:27">
-      <c r="B143" s="128"/>
-      <c r="C143" s="125"/>
-      <c r="E143" s="143"/>
-      <c r="F143" s="148"/>
+      <c r="B143" s="125"/>
+      <c r="C143" s="133"/>
+      <c r="E143" s="117"/>
+      <c r="F143" s="122"/>
       <c r="G143" s="48"/>
       <c r="H143" s="48"/>
       <c r="I143" s="48"/>
@@ -7389,10 +7391,10 @@
       <c r="AA143" s="53"/>
     </row>
     <row r="144" spans="2:27">
-      <c r="B144" s="128"/>
-      <c r="C144" s="125"/>
-      <c r="E144" s="143"/>
-      <c r="F144" s="148"/>
+      <c r="B144" s="125"/>
+      <c r="C144" s="133"/>
+      <c r="E144" s="117"/>
+      <c r="F144" s="122"/>
       <c r="G144" s="48"/>
       <c r="H144" s="48"/>
       <c r="I144" s="48"/>
@@ -7433,11 +7435,11 @@
       <c r="Z144" s="48"/>
       <c r="AA144" s="53"/>
     </row>
-    <row r="145" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B145" s="128"/>
-      <c r="C145" s="125"/>
-      <c r="E145" s="143"/>
-      <c r="F145" s="148"/>
+    <row r="145" spans="2:27" ht="16" customHeight="1">
+      <c r="B145" s="125"/>
+      <c r="C145" s="133"/>
+      <c r="E145" s="117"/>
+      <c r="F145" s="122"/>
       <c r="G145" s="48"/>
       <c r="H145" s="48"/>
       <c r="I145" s="48"/>
@@ -7479,12 +7481,12 @@
       <c r="AA145" s="53"/>
     </row>
     <row r="146" spans="2:27">
-      <c r="B146" s="128" t="s">
+      <c r="B146" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="C146" s="125"/>
-      <c r="E146" s="143"/>
-      <c r="F146" s="148"/>
+      <c r="C146" s="133"/>
+      <c r="E146" s="117"/>
+      <c r="F146" s="122"/>
       <c r="G146" s="48"/>
       <c r="H146" s="48"/>
       <c r="I146" s="48"/>
@@ -7526,10 +7528,10 @@
       <c r="AA146" s="53"/>
     </row>
     <row r="147" spans="2:27">
-      <c r="B147" s="128"/>
-      <c r="C147" s="125"/>
-      <c r="E147" s="143"/>
-      <c r="F147" s="148"/>
+      <c r="B147" s="125"/>
+      <c r="C147" s="133"/>
+      <c r="E147" s="117"/>
+      <c r="F147" s="122"/>
       <c r="G147" s="48"/>
       <c r="H147" s="48"/>
       <c r="I147" s="48"/>
@@ -7571,10 +7573,10 @@
       <c r="AA147" s="53"/>
     </row>
     <row r="148" spans="2:27">
-      <c r="B148" s="128"/>
-      <c r="C148" s="125"/>
-      <c r="E148" s="143"/>
-      <c r="F148" s="148"/>
+      <c r="B148" s="125"/>
+      <c r="C148" s="133"/>
+      <c r="E148" s="117"/>
+      <c r="F148" s="122"/>
       <c r="G148" s="48"/>
       <c r="H148" s="48"/>
       <c r="I148" s="48"/>
@@ -7615,11 +7617,11 @@
       <c r="Z148" s="48"/>
       <c r="AA148" s="53"/>
     </row>
-    <row r="149" spans="2:27" ht="16.05" customHeight="1" thickBot="1">
-      <c r="B149" s="128"/>
-      <c r="C149" s="125"/>
-      <c r="E149" s="146"/>
-      <c r="F149" s="149"/>
+    <row r="149" spans="2:27" ht="16" customHeight="1" thickBot="1">
+      <c r="B149" s="125"/>
+      <c r="C149" s="133"/>
+      <c r="E149" s="120"/>
+      <c r="F149" s="123"/>
       <c r="G149" s="56"/>
       <c r="H149" s="56"/>
       <c r="I149" s="56"/>
@@ -7661,9 +7663,9 @@
       <c r="AA149" s="57"/>
     </row>
     <row r="150" spans="2:27">
-      <c r="B150" s="128"/>
-      <c r="C150" s="125"/>
-      <c r="E150" s="142" t="s">
+      <c r="B150" s="125"/>
+      <c r="C150" s="133"/>
+      <c r="E150" s="116" t="s">
         <v>260</v>
       </c>
       <c r="F150" s="63" t="s">
@@ -7711,9 +7713,9 @@
       <c r="AA150" s="52"/>
     </row>
     <row r="151" spans="2:27">
-      <c r="B151" s="128"/>
-      <c r="C151" s="125"/>
-      <c r="E151" s="143"/>
+      <c r="B151" s="125"/>
+      <c r="C151" s="133"/>
+      <c r="E151" s="117"/>
       <c r="F151" s="60" t="s">
         <v>189</v>
       </c>
@@ -7752,9 +7754,9 @@
       <c r="AA151" s="53"/>
     </row>
     <row r="152" spans="2:27">
-      <c r="B152" s="128"/>
-      <c r="C152" s="125"/>
-      <c r="E152" s="143"/>
+      <c r="B152" s="125"/>
+      <c r="C152" s="133"/>
+      <c r="E152" s="117"/>
       <c r="F152" s="60" t="s">
         <v>190</v>
       </c>
@@ -7798,9 +7800,9 @@
       <c r="AA152" s="53"/>
     </row>
     <row r="153" spans="2:27">
-      <c r="B153" s="128"/>
-      <c r="C153" s="125"/>
-      <c r="E153" s="143"/>
+      <c r="B153" s="125"/>
+      <c r="C153" s="133"/>
+      <c r="E153" s="117"/>
       <c r="F153" s="60" t="s">
         <v>191</v>
       </c>
@@ -7836,13 +7838,13 @@
       <c r="AA153" s="53"/>
     </row>
     <row r="154" spans="2:27">
-      <c r="B154" s="128" t="s">
+      <c r="B154" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="C154" s="125" t="s">
+      <c r="C154" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="E154" s="143"/>
+      <c r="E154" s="117"/>
       <c r="F154" s="60" t="s">
         <v>192</v>
       </c>
@@ -7888,9 +7890,9 @@
       <c r="AA154" s="53"/>
     </row>
     <row r="155" spans="2:27">
-      <c r="B155" s="128"/>
-      <c r="C155" s="125"/>
-      <c r="E155" s="143"/>
+      <c r="B155" s="125"/>
+      <c r="C155" s="133"/>
+      <c r="E155" s="117"/>
       <c r="F155" s="60" t="s">
         <v>193</v>
       </c>
@@ -7936,9 +7938,9 @@
       <c r="AA155" s="53"/>
     </row>
     <row r="156" spans="2:27">
-      <c r="B156" s="128"/>
-      <c r="C156" s="125"/>
-      <c r="E156" s="143"/>
+      <c r="B156" s="125"/>
+      <c r="C156" s="133"/>
+      <c r="E156" s="117"/>
       <c r="F156" s="60" t="s">
         <v>194</v>
       </c>
@@ -7983,14 +7985,14 @@
       <c r="Z156" s="48"/>
       <c r="AA156" s="53"/>
     </row>
-    <row r="157" spans="2:27" ht="16.2" thickBot="1">
-      <c r="B157" s="134" t="s">
+    <row r="157" spans="2:27" ht="17" thickBot="1">
+      <c r="B157" s="140" t="s">
         <v>91</v>
       </c>
-      <c r="C157" s="125" t="s">
+      <c r="C157" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="E157" s="144"/>
+      <c r="E157" s="118"/>
       <c r="F157" s="61" t="s">
         <v>197</v>
       </c>
@@ -8028,12 +8030,12 @@
       <c r="AA157" s="55"/>
     </row>
     <row r="158" spans="2:27">
-      <c r="B158" s="134"/>
-      <c r="C158" s="125"/>
-      <c r="E158" s="145" t="s">
+      <c r="B158" s="140"/>
+      <c r="C158" s="133"/>
+      <c r="E158" s="119" t="s">
         <v>81</v>
       </c>
-      <c r="F158" s="150" t="s">
+      <c r="F158" s="124" t="s">
         <v>272</v>
       </c>
       <c r="G158" s="37">
@@ -8065,10 +8067,10 @@
       <c r="AA158" s="52"/>
     </row>
     <row r="159" spans="2:27">
-      <c r="B159" s="134"/>
-      <c r="C159" s="125"/>
-      <c r="E159" s="143"/>
-      <c r="F159" s="128"/>
+      <c r="B159" s="140"/>
+      <c r="C159" s="133"/>
+      <c r="E159" s="117"/>
+      <c r="F159" s="125"/>
       <c r="G159" s="1">
         <v>1.01435445973261</v>
       </c>
@@ -8098,10 +8100,10 @@
       <c r="AA159" s="53"/>
     </row>
     <row r="160" spans="2:27">
-      <c r="B160" s="134"/>
-      <c r="C160" s="125"/>
-      <c r="E160" s="143"/>
-      <c r="F160" s="128"/>
+      <c r="B160" s="140"/>
+      <c r="C160" s="133"/>
+      <c r="E160" s="117"/>
+      <c r="F160" s="125"/>
       <c r="G160" s="1">
         <v>2.0570279393808799</v>
       </c>
@@ -8130,13 +8132,13 @@
       <c r="Z160" s="48"/>
       <c r="AA160" s="53"/>
     </row>
-    <row r="161" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B161" s="134" t="s">
+    <row r="161" spans="2:27" ht="16" customHeight="1">
+      <c r="B161" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="C161" s="125"/>
-      <c r="E161" s="143"/>
-      <c r="F161" s="128"/>
+      <c r="C161" s="133"/>
+      <c r="E161" s="117"/>
+      <c r="F161" s="125"/>
       <c r="G161" s="1">
         <v>5.0235478806907299</v>
       </c>
@@ -8165,11 +8167,11 @@
       <c r="Z161" s="48"/>
       <c r="AA161" s="53"/>
     </row>
-    <row r="162" spans="2:27" ht="16.2" thickBot="1">
-      <c r="B162" s="134"/>
-      <c r="C162" s="125"/>
-      <c r="E162" s="143"/>
-      <c r="F162" s="129"/>
+    <row r="162" spans="2:27" ht="17" thickBot="1">
+      <c r="B162" s="140"/>
+      <c r="C162" s="133"/>
+      <c r="E162" s="117"/>
+      <c r="F162" s="126"/>
       <c r="G162" s="24">
         <v>16.7844573726926</v>
       </c>
@@ -8199,10 +8201,10 @@
       <c r="AA162" s="55"/>
     </row>
     <row r="163" spans="2:27">
-      <c r="B163" s="134"/>
-      <c r="C163" s="125"/>
-      <c r="E163" s="143"/>
-      <c r="F163" s="150" t="s">
+      <c r="B163" s="140"/>
+      <c r="C163" s="133"/>
+      <c r="E163" s="117"/>
+      <c r="F163" s="124" t="s">
         <v>273</v>
       </c>
       <c r="G163" s="37">
@@ -8234,10 +8236,10 @@
       <c r="AA163" s="52"/>
     </row>
     <row r="164" spans="2:27">
-      <c r="B164" s="134"/>
-      <c r="C164" s="125"/>
-      <c r="E164" s="143"/>
-      <c r="F164" s="128"/>
+      <c r="B164" s="140"/>
+      <c r="C164" s="133"/>
+      <c r="E164" s="117"/>
+      <c r="F164" s="125"/>
       <c r="G164" s="1">
         <v>1.0000384334524699</v>
       </c>
@@ -8267,10 +8269,10 @@
       <c r="AA164" s="53"/>
     </row>
     <row r="165" spans="2:27">
-      <c r="B165" s="134"/>
-      <c r="C165" s="125"/>
-      <c r="E165" s="143"/>
-      <c r="F165" s="128"/>
+      <c r="B165" s="140"/>
+      <c r="C165" s="133"/>
+      <c r="E165" s="117"/>
+      <c r="F165" s="125"/>
       <c r="G165" s="1">
         <v>1.9953111187978001</v>
       </c>
@@ -8300,10 +8302,10 @@
       <c r="AA165" s="53"/>
     </row>
     <row r="166" spans="2:27">
-      <c r="B166" s="134"/>
-      <c r="C166" s="125"/>
-      <c r="E166" s="143"/>
-      <c r="F166" s="128"/>
+      <c r="B166" s="140"/>
+      <c r="C166" s="133"/>
+      <c r="E166" s="117"/>
+      <c r="F166" s="125"/>
       <c r="G166" s="1">
         <v>4.9786694338752397</v>
       </c>
@@ -8332,11 +8334,11 @@
       <c r="Z166" s="48"/>
       <c r="AA166" s="53"/>
     </row>
-    <row r="167" spans="2:27" ht="16.2" thickBot="1">
-      <c r="B167" s="134"/>
-      <c r="C167" s="125"/>
-      <c r="E167" s="146"/>
-      <c r="F167" s="129"/>
+    <row r="167" spans="2:27" ht="17" thickBot="1">
+      <c r="B167" s="140"/>
+      <c r="C167" s="133"/>
+      <c r="E167" s="120"/>
+      <c r="F167" s="126"/>
       <c r="G167" s="24">
         <v>16.686933907272799</v>
       </c>
@@ -8366,9 +8368,9 @@
       <c r="AA167" s="55"/>
     </row>
     <row r="168" spans="2:27">
-      <c r="B168" s="134"/>
-      <c r="C168" s="125"/>
-      <c r="E168" s="142" t="s">
+      <c r="B168" s="140"/>
+      <c r="C168" s="133"/>
+      <c r="E168" s="116" t="s">
         <v>105</v>
       </c>
       <c r="F168" s="64"/>
@@ -8404,13 +8406,13 @@
       </c>
     </row>
     <row r="169" spans="2:27">
-      <c r="B169" s="128" t="s">
+      <c r="B169" s="125" t="s">
         <v>95</v>
       </c>
-      <c r="C169" s="125" t="s">
+      <c r="C169" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="E169" s="143"/>
+      <c r="E169" s="117"/>
       <c r="F169" s="65"/>
       <c r="G169" s="48"/>
       <c r="H169" s="48"/>
@@ -8444,9 +8446,9 @@
       </c>
     </row>
     <row r="170" spans="2:27">
-      <c r="B170" s="128"/>
-      <c r="C170" s="125"/>
-      <c r="E170" s="143"/>
+      <c r="B170" s="125"/>
+      <c r="C170" s="133"/>
+      <c r="E170" s="117"/>
       <c r="F170" s="65"/>
       <c r="G170" s="48"/>
       <c r="H170" s="48"/>
@@ -8480,9 +8482,9 @@
       </c>
     </row>
     <row r="171" spans="2:27">
-      <c r="B171" s="128"/>
-      <c r="C171" s="125"/>
-      <c r="E171" s="143"/>
+      <c r="B171" s="125"/>
+      <c r="C171" s="133"/>
+      <c r="E171" s="117"/>
       <c r="F171" s="65"/>
       <c r="G171" s="48"/>
       <c r="H171" s="48"/>
@@ -8515,10 +8517,10 @@
         <v>19.922371500000001</v>
       </c>
     </row>
-    <row r="172" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B172" s="128"/>
-      <c r="C172" s="125"/>
-      <c r="E172" s="143"/>
+    <row r="172" spans="2:27" ht="16" customHeight="1">
+      <c r="B172" s="125"/>
+      <c r="C172" s="133"/>
+      <c r="E172" s="117"/>
       <c r="F172" s="65"/>
       <c r="G172" s="48"/>
       <c r="H172" s="48"/>
@@ -8552,13 +8554,13 @@
       </c>
     </row>
     <row r="173" spans="2:27">
-      <c r="B173" s="128" t="s">
+      <c r="B173" s="125" t="s">
         <v>97</v>
       </c>
-      <c r="C173" s="125" t="s">
+      <c r="C173" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="E173" s="143"/>
+      <c r="E173" s="117"/>
       <c r="F173" s="65"/>
       <c r="G173" s="48"/>
       <c r="H173" s="48"/>
@@ -8592,9 +8594,9 @@
       </c>
     </row>
     <row r="174" spans="2:27">
-      <c r="B174" s="128"/>
-      <c r="C174" s="125"/>
-      <c r="E174" s="143"/>
+      <c r="B174" s="125"/>
+      <c r="C174" s="133"/>
+      <c r="E174" s="117"/>
       <c r="F174" s="65"/>
       <c r="G174" s="48"/>
       <c r="H174" s="48"/>
@@ -8628,9 +8630,9 @@
       </c>
     </row>
     <row r="175" spans="2:27">
-      <c r="B175" s="128"/>
-      <c r="C175" s="125"/>
-      <c r="E175" s="143"/>
+      <c r="B175" s="125"/>
+      <c r="C175" s="133"/>
+      <c r="E175" s="117"/>
       <c r="F175" s="65"/>
       <c r="G175" s="48"/>
       <c r="H175" s="48"/>
@@ -8664,9 +8666,9 @@
       </c>
     </row>
     <row r="176" spans="2:27">
-      <c r="B176" s="128"/>
-      <c r="C176" s="125"/>
-      <c r="E176" s="143"/>
+      <c r="B176" s="125"/>
+      <c r="C176" s="133"/>
+      <c r="E176" s="117"/>
       <c r="F176" s="65"/>
       <c r="G176" s="48"/>
       <c r="H176" s="48"/>
@@ -8700,11 +8702,11 @@
       </c>
     </row>
     <row r="177" spans="2:27">
-      <c r="B177" s="128" t="s">
+      <c r="B177" s="125" t="s">
         <v>98</v>
       </c>
-      <c r="C177" s="125"/>
-      <c r="E177" s="143"/>
+      <c r="C177" s="133"/>
+      <c r="E177" s="117"/>
       <c r="F177" s="65"/>
       <c r="G177" s="48"/>
       <c r="H177" s="48"/>
@@ -8738,9 +8740,9 @@
       </c>
     </row>
     <row r="178" spans="2:27">
-      <c r="B178" s="128"/>
-      <c r="C178" s="125"/>
-      <c r="E178" s="143"/>
+      <c r="B178" s="125"/>
+      <c r="C178" s="133"/>
+      <c r="E178" s="117"/>
       <c r="F178" s="65"/>
       <c r="G178" s="48"/>
       <c r="H178" s="48"/>
@@ -8774,9 +8776,9 @@
       </c>
     </row>
     <row r="179" spans="2:27">
-      <c r="B179" s="128"/>
-      <c r="C179" s="125"/>
-      <c r="E179" s="143"/>
+      <c r="B179" s="125"/>
+      <c r="C179" s="133"/>
+      <c r="E179" s="117"/>
       <c r="F179" s="65"/>
       <c r="G179" s="48"/>
       <c r="H179" s="48"/>
@@ -8809,10 +8811,10 @@
         <v>30.0627073</v>
       </c>
     </row>
-    <row r="180" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B180" s="128"/>
-      <c r="C180" s="125"/>
-      <c r="E180" s="143"/>
+    <row r="180" spans="2:27" ht="16" customHeight="1">
+      <c r="B180" s="125"/>
+      <c r="C180" s="133"/>
+      <c r="E180" s="117"/>
       <c r="F180" s="65"/>
       <c r="G180" s="48"/>
       <c r="H180" s="48"/>
@@ -8846,13 +8848,13 @@
       </c>
     </row>
     <row r="181" spans="2:27">
-      <c r="B181" s="128" t="s">
+      <c r="B181" s="125" t="s">
         <v>99</v>
       </c>
-      <c r="C181" s="125" t="s">
+      <c r="C181" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="E181" s="143"/>
+      <c r="E181" s="117"/>
       <c r="F181" s="65"/>
       <c r="G181" s="48"/>
       <c r="H181" s="48"/>
@@ -8886,9 +8888,9 @@
       </c>
     </row>
     <row r="182" spans="2:27">
-      <c r="B182" s="128"/>
-      <c r="C182" s="125"/>
-      <c r="E182" s="143"/>
+      <c r="B182" s="125"/>
+      <c r="C182" s="133"/>
+      <c r="E182" s="117"/>
       <c r="F182" s="65"/>
       <c r="G182" s="48"/>
       <c r="H182" s="48"/>
@@ -8928,7 +8930,7 @@
       <c r="C183" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E183" s="143"/>
+      <c r="E183" s="117"/>
       <c r="F183" s="65"/>
       <c r="G183" s="48"/>
       <c r="H183" s="48"/>
@@ -8962,13 +8964,13 @@
       </c>
     </row>
     <row r="184" spans="2:27">
-      <c r="B184" s="128" t="s">
+      <c r="B184" s="125" t="s">
         <v>103</v>
       </c>
-      <c r="C184" s="125" t="s">
+      <c r="C184" s="133" t="s">
         <v>102</v>
       </c>
-      <c r="E184" s="143"/>
+      <c r="E184" s="117"/>
       <c r="F184" s="65"/>
       <c r="G184" s="48"/>
       <c r="H184" s="48"/>
@@ -9002,9 +9004,9 @@
       </c>
     </row>
     <row r="185" spans="2:27">
-      <c r="B185" s="128"/>
-      <c r="C185" s="125"/>
-      <c r="E185" s="143"/>
+      <c r="B185" s="125"/>
+      <c r="C185" s="133"/>
+      <c r="E185" s="117"/>
       <c r="F185" s="65"/>
       <c r="G185" s="48"/>
       <c r="H185" s="48"/>
@@ -9037,10 +9039,10 @@
         <v>40.4672141</v>
       </c>
     </row>
-    <row r="186" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B186" s="128"/>
-      <c r="C186" s="125"/>
-      <c r="E186" s="143"/>
+    <row r="186" spans="2:27" ht="16" customHeight="1">
+      <c r="B186" s="125"/>
+      <c r="C186" s="133"/>
+      <c r="E186" s="117"/>
       <c r="F186" s="65"/>
       <c r="G186" s="48"/>
       <c r="H186" s="48"/>
@@ -9074,9 +9076,9 @@
       </c>
     </row>
     <row r="187" spans="2:27">
-      <c r="B187" s="128"/>
-      <c r="C187" s="125"/>
-      <c r="E187" s="143"/>
+      <c r="B187" s="125"/>
+      <c r="C187" s="133"/>
+      <c r="E187" s="117"/>
       <c r="F187" s="65"/>
       <c r="G187" s="48"/>
       <c r="H187" s="48"/>
@@ -9110,9 +9112,9 @@
       </c>
     </row>
     <row r="188" spans="2:27">
-      <c r="B188" s="128"/>
-      <c r="C188" s="125"/>
-      <c r="E188" s="143"/>
+      <c r="B188" s="125"/>
+      <c r="C188" s="133"/>
+      <c r="E188" s="117"/>
       <c r="F188" s="65"/>
       <c r="G188" s="48"/>
       <c r="H188" s="48"/>
@@ -9145,10 +9147,10 @@
         <v>44.019746099999999</v>
       </c>
     </row>
-    <row r="189" spans="2:27" ht="16.2" thickBot="1">
-      <c r="B189" s="128"/>
-      <c r="C189" s="125"/>
-      <c r="E189" s="144"/>
+    <row r="189" spans="2:27" ht="17" thickBot="1">
+      <c r="B189" s="125"/>
+      <c r="C189" s="133"/>
+      <c r="E189" s="118"/>
       <c r="F189" s="66"/>
       <c r="G189" s="54"/>
       <c r="H189" s="54"/>
@@ -9181,53 +9183,53 @@
         <v>43.709449900000003</v>
       </c>
     </row>
-    <row r="190" spans="2:27" ht="16.05" customHeight="1">
-      <c r="B190" s="128" t="s">
+    <row r="190" spans="2:27" ht="16" customHeight="1">
+      <c r="B190" s="125" t="s">
         <v>112</v>
       </c>
-      <c r="C190" s="125"/>
+      <c r="C190" s="133"/>
     </row>
     <row r="191" spans="2:27">
-      <c r="B191" s="128"/>
-      <c r="C191" s="125"/>
+      <c r="B191" s="125"/>
+      <c r="C191" s="133"/>
     </row>
     <row r="192" spans="2:27">
-      <c r="B192" s="128"/>
-      <c r="C192" s="125"/>
+      <c r="B192" s="125"/>
+      <c r="C192" s="133"/>
     </row>
     <row r="193" spans="2:5">
-      <c r="B193" s="128"/>
-      <c r="C193" s="125"/>
+      <c r="B193" s="125"/>
+      <c r="C193" s="133"/>
     </row>
     <row r="194" spans="2:5">
-      <c r="B194" s="128" t="s">
+      <c r="B194" s="125" t="s">
         <v>104</v>
       </c>
-      <c r="C194" s="125" t="s">
+      <c r="C194" s="133" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="195" spans="2:5">
-      <c r="B195" s="128"/>
-      <c r="C195" s="125"/>
+      <c r="B195" s="125"/>
+      <c r="C195" s="133"/>
     </row>
     <row r="196" spans="2:5">
-      <c r="B196" s="133" t="s">
+      <c r="B196" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="C196" s="125" t="s">
+      <c r="C196" s="133" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="197" spans="2:5">
-      <c r="B197" s="133"/>
-      <c r="C197" s="125"/>
+      <c r="B197" s="144"/>
+      <c r="C197" s="133"/>
     </row>
     <row r="198" spans="2:5">
-      <c r="B198" s="128" t="s">
+      <c r="B198" s="125" t="s">
         <v>111</v>
       </c>
-      <c r="C198" s="125" t="s">
+      <c r="C198" s="133" t="s">
         <v>110</v>
       </c>
       <c r="E198" s="47" t="s">
@@ -9235,109 +9237,109 @@
       </c>
     </row>
     <row r="199" spans="2:5">
-      <c r="B199" s="128"/>
-      <c r="C199" s="125"/>
+      <c r="B199" s="125"/>
+      <c r="C199" s="133"/>
       <c r="E199" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="200" spans="2:5">
-      <c r="B200" s="128"/>
-      <c r="C200" s="125"/>
-    </row>
-    <row r="201" spans="2:5" ht="16.05" customHeight="1">
-      <c r="B201" s="128"/>
-      <c r="C201" s="125"/>
+      <c r="B200" s="125"/>
+      <c r="C200" s="133"/>
+    </row>
+    <row r="201" spans="2:5" ht="16" customHeight="1">
+      <c r="B201" s="125"/>
+      <c r="C201" s="133"/>
     </row>
     <row r="202" spans="2:5">
-      <c r="B202" s="128"/>
-      <c r="C202" s="125"/>
-    </row>
-    <row r="203" spans="2:5" ht="16.05" customHeight="1">
-      <c r="B203" s="128"/>
-      <c r="C203" s="125"/>
+      <c r="B202" s="125"/>
+      <c r="C202" s="133"/>
+    </row>
+    <row r="203" spans="2:5" ht="16" customHeight="1">
+      <c r="B203" s="125"/>
+      <c r="C203" s="133"/>
     </row>
     <row r="204" spans="2:5">
-      <c r="B204" s="128"/>
-      <c r="C204" s="125"/>
+      <c r="B204" s="125"/>
+      <c r="C204" s="133"/>
     </row>
     <row r="205" spans="2:5">
-      <c r="B205" s="128" t="s">
+      <c r="B205" s="125" t="s">
         <v>121</v>
       </c>
-      <c r="C205" s="125" t="s">
+      <c r="C205" s="133" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="206" spans="2:5">
-      <c r="B206" s="128"/>
-      <c r="C206" s="125"/>
+      <c r="B206" s="125"/>
+      <c r="C206" s="133"/>
     </row>
     <row r="207" spans="2:5">
-      <c r="B207" s="128"/>
-      <c r="C207" s="125"/>
+      <c r="B207" s="125"/>
+      <c r="C207" s="133"/>
     </row>
     <row r="208" spans="2:5">
-      <c r="B208" s="128" t="s">
+      <c r="B208" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="C208" s="125" t="s">
+      <c r="C208" s="133" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="209" spans="2:3">
-      <c r="B209" s="128"/>
-      <c r="C209" s="125"/>
+      <c r="B209" s="125"/>
+      <c r="C209" s="133"/>
     </row>
     <row r="210" spans="2:3">
-      <c r="B210" s="128" t="s">
+      <c r="B210" s="125" t="s">
         <v>114</v>
       </c>
-      <c r="C210" s="125" t="s">
+      <c r="C210" s="133" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="211" spans="2:3">
-      <c r="B211" s="128"/>
-      <c r="C211" s="125"/>
+      <c r="B211" s="125"/>
+      <c r="C211" s="133"/>
     </row>
     <row r="212" spans="2:3">
-      <c r="B212" s="128"/>
-      <c r="C212" s="125"/>
+      <c r="B212" s="125"/>
+      <c r="C212" s="133"/>
     </row>
     <row r="213" spans="2:3">
-      <c r="B213" s="128" t="s">
+      <c r="B213" s="125" t="s">
         <v>117</v>
       </c>
-      <c r="C213" s="125"/>
+      <c r="C213" s="133"/>
     </row>
     <row r="214" spans="2:3">
-      <c r="B214" s="128"/>
-      <c r="C214" s="125"/>
+      <c r="B214" s="125"/>
+      <c r="C214" s="133"/>
     </row>
     <row r="215" spans="2:3">
-      <c r="B215" s="128" t="s">
+      <c r="B215" s="125" t="s">
         <v>118</v>
       </c>
-      <c r="C215" s="125"/>
-    </row>
-    <row r="216" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B216" s="128"/>
-      <c r="C216" s="125"/>
+      <c r="C215" s="133"/>
+    </row>
+    <row r="216" spans="2:3" ht="16" customHeight="1">
+      <c r="B216" s="125"/>
+      <c r="C216" s="133"/>
     </row>
     <row r="217" spans="2:3">
-      <c r="B217" s="128" t="s">
+      <c r="B217" s="125" t="s">
         <v>119</v>
       </c>
-      <c r="C217" s="125" t="s">
+      <c r="C217" s="133" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="218" spans="2:3" ht="16.2" thickBot="1">
-      <c r="B218" s="128"/>
-      <c r="C218" s="125"/>
-    </row>
-    <row r="219" spans="2:3" ht="16.2" thickBot="1">
+    <row r="218" spans="2:3" ht="17" thickBot="1">
+      <c r="B218" s="125"/>
+      <c r="C218" s="133"/>
+    </row>
+    <row r="219" spans="2:3" ht="17" thickBot="1">
       <c r="B219" s="18" t="s">
         <v>123</v>
       </c>
@@ -9346,336 +9348,336 @@
       </c>
     </row>
     <row r="220" spans="2:3">
-      <c r="B220" s="127" t="s">
+      <c r="B220" s="130" t="s">
         <v>125</v>
       </c>
-      <c r="C220" s="124" t="s">
+      <c r="C220" s="138" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="221" spans="2:3">
-      <c r="B221" s="128"/>
-      <c r="C221" s="125"/>
+      <c r="B221" s="125"/>
+      <c r="C221" s="133"/>
     </row>
     <row r="222" spans="2:3">
-      <c r="B222" s="128"/>
-      <c r="C222" s="125"/>
+      <c r="B222" s="125"/>
+      <c r="C222" s="133"/>
     </row>
     <row r="223" spans="2:3">
-      <c r="B223" s="128"/>
-      <c r="C223" s="125"/>
+      <c r="B223" s="125"/>
+      <c r="C223" s="133"/>
     </row>
     <row r="224" spans="2:3">
-      <c r="B224" s="128"/>
-      <c r="C224" s="125"/>
-    </row>
-    <row r="225" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B225" s="128"/>
-      <c r="C225" s="125"/>
+      <c r="B224" s="125"/>
+      <c r="C224" s="133"/>
+    </row>
+    <row r="225" spans="2:3" ht="16" customHeight="1">
+      <c r="B225" s="125"/>
+      <c r="C225" s="133"/>
     </row>
     <row r="226" spans="2:3">
-      <c r="B226" s="128"/>
-      <c r="C226" s="125"/>
-    </row>
-    <row r="227" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B227" s="128" t="s">
+      <c r="B226" s="125"/>
+      <c r="C226" s="133"/>
+    </row>
+    <row r="227" spans="2:3" ht="16" customHeight="1">
+      <c r="B227" s="125" t="s">
         <v>127</v>
       </c>
-      <c r="C227" s="125"/>
+      <c r="C227" s="133"/>
     </row>
     <row r="228" spans="2:3">
-      <c r="B228" s="131"/>
-      <c r="C228" s="132"/>
+      <c r="B228" s="143"/>
+      <c r="C228" s="141"/>
     </row>
     <row r="229" spans="2:3">
-      <c r="B229" s="128" t="s">
+      <c r="B229" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="C229" s="125" t="s">
+      <c r="C229" s="133" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="230" spans="2:3">
-      <c r="B230" s="128"/>
-      <c r="C230" s="125"/>
+      <c r="B230" s="125"/>
+      <c r="C230" s="133"/>
     </row>
     <row r="231" spans="2:3">
-      <c r="B231" s="128" t="s">
+      <c r="B231" s="125" t="s">
         <v>131</v>
       </c>
-      <c r="C231" s="125"/>
+      <c r="C231" s="133"/>
     </row>
     <row r="232" spans="2:3">
-      <c r="B232" s="128"/>
-      <c r="C232" s="125"/>
+      <c r="B232" s="125"/>
+      <c r="C232" s="133"/>
     </row>
     <row r="233" spans="2:3">
-      <c r="B233" s="128"/>
-      <c r="C233" s="125"/>
+      <c r="B233" s="125"/>
+      <c r="C233" s="133"/>
     </row>
     <row r="234" spans="2:3">
-      <c r="B234" s="128"/>
-      <c r="C234" s="125"/>
+      <c r="B234" s="125"/>
+      <c r="C234" s="133"/>
     </row>
     <row r="235" spans="2:3">
-      <c r="B235" s="128"/>
-      <c r="C235" s="125"/>
+      <c r="B235" s="125"/>
+      <c r="C235" s="133"/>
     </row>
     <row r="236" spans="2:3">
-      <c r="B236" s="128"/>
-      <c r="C236" s="125"/>
+      <c r="B236" s="125"/>
+      <c r="C236" s="133"/>
     </row>
     <row r="237" spans="2:3">
-      <c r="B237" s="128"/>
-      <c r="C237" s="125"/>
+      <c r="B237" s="125"/>
+      <c r="C237" s="133"/>
     </row>
     <row r="238" spans="2:3">
-      <c r="B238" s="128"/>
-      <c r="C238" s="125"/>
+      <c r="B238" s="125"/>
+      <c r="C238" s="133"/>
     </row>
     <row r="239" spans="2:3">
-      <c r="B239" s="128"/>
-      <c r="C239" s="125"/>
-    </row>
-    <row r="240" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B240" s="128" t="s">
+      <c r="B239" s="125"/>
+      <c r="C239" s="133"/>
+    </row>
+    <row r="240" spans="2:3" ht="16" customHeight="1">
+      <c r="B240" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="C240" s="125" t="s">
+      <c r="C240" s="133" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="241" spans="2:3">
-      <c r="B241" s="128"/>
-      <c r="C241" s="125"/>
+      <c r="B241" s="125"/>
+      <c r="C241" s="133"/>
     </row>
     <row r="242" spans="2:3">
-      <c r="B242" s="128" t="s">
+      <c r="B242" s="125" t="s">
         <v>133</v>
       </c>
-      <c r="C242" s="125" t="s">
+      <c r="C242" s="133" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="243" spans="2:3">
-      <c r="B243" s="128"/>
-      <c r="C243" s="125"/>
-    </row>
-    <row r="244" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B244" s="128" t="s">
+      <c r="B243" s="125"/>
+      <c r="C243" s="133"/>
+    </row>
+    <row r="244" spans="2:3" ht="16" customHeight="1">
+      <c r="B244" s="125" t="s">
         <v>134</v>
       </c>
-      <c r="C244" s="125" t="s">
+      <c r="C244" s="133" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="245" spans="2:3">
-      <c r="B245" s="128"/>
-      <c r="C245" s="125"/>
-    </row>
-    <row r="246" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B246" s="128"/>
-      <c r="C246" s="125"/>
+      <c r="B245" s="125"/>
+      <c r="C245" s="133"/>
+    </row>
+    <row r="246" spans="2:3" ht="16" customHeight="1">
+      <c r="B246" s="125"/>
+      <c r="C246" s="133"/>
     </row>
     <row r="247" spans="2:3">
-      <c r="B247" s="128"/>
-      <c r="C247" s="125"/>
+      <c r="B247" s="125"/>
+      <c r="C247" s="133"/>
     </row>
     <row r="248" spans="2:3">
-      <c r="B248" s="128" t="s">
+      <c r="B248" s="125" t="s">
         <v>136</v>
       </c>
-      <c r="C248" s="125" t="s">
+      <c r="C248" s="133" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="249" spans="2:3">
-      <c r="B249" s="128"/>
-      <c r="C249" s="125"/>
+      <c r="B249" s="125"/>
+      <c r="C249" s="133"/>
     </row>
     <row r="250" spans="2:3">
-      <c r="B250" s="128" t="s">
+      <c r="B250" s="125" t="s">
         <v>138</v>
       </c>
-      <c r="C250" s="125"/>
+      <c r="C250" s="133"/>
     </row>
     <row r="251" spans="2:3">
-      <c r="B251" s="128"/>
-      <c r="C251" s="125"/>
+      <c r="B251" s="125"/>
+      <c r="C251" s="133"/>
     </row>
     <row r="252" spans="2:3">
-      <c r="B252" s="128"/>
-      <c r="C252" s="125"/>
-    </row>
-    <row r="253" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B253" s="128"/>
-      <c r="C253" s="125"/>
+      <c r="B252" s="125"/>
+      <c r="C252" s="133"/>
+    </row>
+    <row r="253" spans="2:3" ht="16" customHeight="1">
+      <c r="B253" s="125"/>
+      <c r="C253" s="133"/>
     </row>
     <row r="254" spans="2:3">
-      <c r="B254" s="128"/>
-      <c r="C254" s="125"/>
+      <c r="B254" s="125"/>
+      <c r="C254" s="133"/>
     </row>
     <row r="255" spans="2:3">
-      <c r="B255" s="128"/>
-      <c r="C255" s="125"/>
+      <c r="B255" s="125"/>
+      <c r="C255" s="133"/>
     </row>
     <row r="256" spans="2:3">
-      <c r="B256" s="128"/>
-      <c r="C256" s="125"/>
-    </row>
-    <row r="257" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B257" s="128" t="s">
+      <c r="B256" s="125"/>
+      <c r="C256" s="133"/>
+    </row>
+    <row r="257" spans="2:3" ht="16" customHeight="1">
+      <c r="B257" s="125" t="s">
         <v>139</v>
       </c>
-      <c r="C257" s="125"/>
+      <c r="C257" s="133"/>
     </row>
     <row r="258" spans="2:3">
-      <c r="B258" s="128"/>
-      <c r="C258" s="125"/>
+      <c r="B258" s="125"/>
+      <c r="C258" s="133"/>
     </row>
     <row r="259" spans="2:3">
-      <c r="B259" s="128"/>
-      <c r="C259" s="125"/>
+      <c r="B259" s="125"/>
+      <c r="C259" s="133"/>
     </row>
     <row r="260" spans="2:3">
-      <c r="B260" s="128"/>
-      <c r="C260" s="125"/>
+      <c r="B260" s="125"/>
+      <c r="C260" s="133"/>
     </row>
     <row r="261" spans="2:3">
-      <c r="B261" s="128" t="s">
+      <c r="B261" s="125" t="s">
         <v>141</v>
       </c>
-      <c r="C261" s="125"/>
-    </row>
-    <row r="262" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B262" s="128"/>
-      <c r="C262" s="125"/>
+      <c r="C261" s="133"/>
+    </row>
+    <row r="262" spans="2:3" ht="16" customHeight="1">
+      <c r="B262" s="125"/>
+      <c r="C262" s="133"/>
     </row>
     <row r="263" spans="2:3">
-      <c r="B263" s="128" t="s">
+      <c r="B263" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="C263" s="125" t="s">
+      <c r="C263" s="133" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="264" spans="2:3">
-      <c r="B264" s="128"/>
-      <c r="C264" s="125"/>
+      <c r="B264" s="125"/>
+      <c r="C264" s="133"/>
     </row>
     <row r="265" spans="2:3">
-      <c r="B265" s="128"/>
-      <c r="C265" s="125"/>
+      <c r="B265" s="125"/>
+      <c r="C265" s="133"/>
     </row>
     <row r="266" spans="2:3">
-      <c r="B266" s="128" t="s">
+      <c r="B266" s="125" t="s">
         <v>142</v>
       </c>
-      <c r="C266" s="125" t="s">
+      <c r="C266" s="133" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="267" spans="2:3">
-      <c r="B267" s="128"/>
-      <c r="C267" s="125"/>
-    </row>
-    <row r="268" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B268" s="128"/>
-      <c r="C268" s="125"/>
+      <c r="B267" s="125"/>
+      <c r="C267" s="133"/>
+    </row>
+    <row r="268" spans="2:3" ht="16" customHeight="1">
+      <c r="B268" s="125"/>
+      <c r="C268" s="133"/>
     </row>
     <row r="269" spans="2:3">
-      <c r="B269" s="128"/>
-      <c r="C269" s="125"/>
+      <c r="B269" s="125"/>
+      <c r="C269" s="133"/>
     </row>
     <row r="270" spans="2:3">
-      <c r="B270" s="128" t="s">
+      <c r="B270" s="125" t="s">
         <v>144</v>
       </c>
-      <c r="C270" s="125" t="s">
+      <c r="C270" s="133" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="271" spans="2:3" ht="18" customHeight="1">
-      <c r="B271" s="128"/>
-      <c r="C271" s="125"/>
+      <c r="B271" s="125"/>
+      <c r="C271" s="133"/>
     </row>
     <row r="272" spans="2:3">
-      <c r="B272" s="128" t="s">
+      <c r="B272" s="125" t="s">
         <v>146</v>
       </c>
-      <c r="C272" s="125" t="s">
+      <c r="C272" s="133" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="273" spans="2:3">
-      <c r="B273" s="128"/>
-      <c r="C273" s="125"/>
+      <c r="B273" s="125"/>
+      <c r="C273" s="133"/>
     </row>
     <row r="274" spans="2:3">
-      <c r="B274" s="128"/>
-      <c r="C274" s="125"/>
+      <c r="B274" s="125"/>
+      <c r="C274" s="133"/>
     </row>
     <row r="275" spans="2:3">
-      <c r="B275" s="128" t="s">
+      <c r="B275" s="125" t="s">
         <v>149</v>
       </c>
-      <c r="C275" s="125" t="s">
+      <c r="C275" s="133" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="276" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B276" s="128"/>
-      <c r="C276" s="125"/>
+    <row r="276" spans="2:3" ht="16" customHeight="1">
+      <c r="B276" s="125"/>
+      <c r="C276" s="133"/>
     </row>
     <row r="277" spans="2:3">
-      <c r="B277" s="128"/>
-      <c r="C277" s="125"/>
+      <c r="B277" s="125"/>
+      <c r="C277" s="133"/>
     </row>
     <row r="278" spans="2:3">
-      <c r="B278" s="128" t="s">
+      <c r="B278" s="125" t="s">
         <v>150</v>
       </c>
-      <c r="C278" s="125" t="s">
+      <c r="C278" s="133" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="279" spans="2:3">
-      <c r="B279" s="128"/>
-      <c r="C279" s="125"/>
+      <c r="B279" s="125"/>
+      <c r="C279" s="133"/>
     </row>
     <row r="280" spans="2:3">
-      <c r="B280" s="128" t="s">
+      <c r="B280" s="125" t="s">
         <v>152</v>
       </c>
-      <c r="C280" s="125" t="s">
+      <c r="C280" s="133" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="281" spans="2:3">
-      <c r="B281" s="128"/>
-      <c r="C281" s="125"/>
+      <c r="B281" s="125"/>
+      <c r="C281" s="133"/>
     </row>
     <row r="282" spans="2:3">
-      <c r="B282" s="128"/>
-      <c r="C282" s="125"/>
-    </row>
-    <row r="283" spans="2:3" ht="16.05" customHeight="1">
-      <c r="B283" s="128"/>
-      <c r="C283" s="125"/>
+      <c r="B282" s="125"/>
+      <c r="C282" s="133"/>
+    </row>
+    <row r="283" spans="2:3" ht="16" customHeight="1">
+      <c r="B283" s="125"/>
+      <c r="C283" s="133"/>
     </row>
     <row r="284" spans="2:3">
-      <c r="B284" s="128" t="s">
+      <c r="B284" s="125" t="s">
         <v>154</v>
       </c>
-      <c r="C284" s="125" t="s">
+      <c r="C284" s="133" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="285" spans="2:3" ht="16.2" thickBot="1">
-      <c r="B285" s="128"/>
-      <c r="C285" s="125"/>
-    </row>
-    <row r="286" spans="2:3" ht="16.2" thickBot="1">
+    <row r="285" spans="2:3" ht="17" thickBot="1">
+      <c r="B285" s="125"/>
+      <c r="C285" s="133"/>
+    </row>
+    <row r="286" spans="2:3" ht="17" thickBot="1">
       <c r="B286" s="18" t="s">
         <v>158</v>
       </c>
@@ -9684,152 +9686,48 @@
       </c>
     </row>
     <row r="287" spans="2:3">
-      <c r="B287" s="127" t="s">
+      <c r="B287" s="130" t="s">
         <v>157</v>
       </c>
-      <c r="C287" s="124" t="s">
+      <c r="C287" s="138" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="288" spans="2:3">
-      <c r="B288" s="128"/>
-      <c r="C288" s="125"/>
+      <c r="B288" s="125"/>
+      <c r="C288" s="133"/>
     </row>
     <row r="289" spans="2:3">
-      <c r="B289" s="128"/>
-      <c r="C289" s="125" t="s">
+      <c r="B289" s="125"/>
+      <c r="C289" s="133" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="290" spans="2:3">
-      <c r="B290" s="128"/>
-      <c r="C290" s="125"/>
-    </row>
-    <row r="291" spans="2:3" ht="16.2" thickBot="1">
-      <c r="B291" s="129"/>
-      <c r="C291" s="126"/>
+      <c r="B290" s="125"/>
+      <c r="C290" s="133"/>
+    </row>
+    <row r="291" spans="2:3" ht="17" thickBot="1">
+      <c r="B291" s="126"/>
+      <c r="C291" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="158">
-    <mergeCell ref="E168:E189"/>
-    <mergeCell ref="E103:E113"/>
-    <mergeCell ref="E150:E157"/>
-    <mergeCell ref="E114:E149"/>
-    <mergeCell ref="F114:F149"/>
-    <mergeCell ref="F158:F162"/>
-    <mergeCell ref="F163:F167"/>
-    <mergeCell ref="E158:E167"/>
-    <mergeCell ref="E101:AA101"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B44:B51"/>
-    <mergeCell ref="C44:C51"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="C38:C43"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B73:B77"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C68:C72"/>
-    <mergeCell ref="B68:B72"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="C126:C128"/>
-    <mergeCell ref="B124:B128"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="B107:B113"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="B116:B119"/>
-    <mergeCell ref="C107:C119"/>
-    <mergeCell ref="B177:B180"/>
-    <mergeCell ref="C173:C180"/>
-    <mergeCell ref="B181:B182"/>
-    <mergeCell ref="C181:C182"/>
-    <mergeCell ref="B161:B168"/>
-    <mergeCell ref="C157:C168"/>
-    <mergeCell ref="B169:B172"/>
-    <mergeCell ref="C169:C172"/>
-    <mergeCell ref="B173:B176"/>
-    <mergeCell ref="B146:B153"/>
-    <mergeCell ref="C141:C153"/>
-    <mergeCell ref="C154:C156"/>
-    <mergeCell ref="B154:B156"/>
-    <mergeCell ref="B157:B160"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B133:B135"/>
-    <mergeCell ref="C133:C135"/>
-    <mergeCell ref="B136:B140"/>
-    <mergeCell ref="C136:C140"/>
-    <mergeCell ref="B141:B145"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="C129:C132"/>
-    <mergeCell ref="B220:B226"/>
-    <mergeCell ref="B227:B228"/>
-    <mergeCell ref="C220:C228"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="B215:B216"/>
-    <mergeCell ref="C210:C216"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="B217:B218"/>
-    <mergeCell ref="B190:B193"/>
-    <mergeCell ref="C184:C193"/>
-    <mergeCell ref="B210:B212"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:C209"/>
-    <mergeCell ref="B205:B207"/>
-    <mergeCell ref="C205:C207"/>
-    <mergeCell ref="C196:C197"/>
-    <mergeCell ref="B196:B197"/>
-    <mergeCell ref="B198:B204"/>
-    <mergeCell ref="C198:C204"/>
-    <mergeCell ref="B194:B195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="B184:B189"/>
-    <mergeCell ref="C242:C243"/>
-    <mergeCell ref="B242:B243"/>
-    <mergeCell ref="B244:B247"/>
-    <mergeCell ref="C244:C247"/>
-    <mergeCell ref="B248:B249"/>
-    <mergeCell ref="B229:B230"/>
-    <mergeCell ref="C240:C241"/>
-    <mergeCell ref="B240:B241"/>
-    <mergeCell ref="B231:B239"/>
-    <mergeCell ref="C229:C239"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="E68:H68"/>
+    <mergeCell ref="E82:H82"/>
+    <mergeCell ref="E84:H84"/>
+    <mergeCell ref="E90:H90"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E34:H34"/>
     <mergeCell ref="C287:C288"/>
     <mergeCell ref="C289:C291"/>
     <mergeCell ref="B287:B291"/>
@@ -9854,21 +9752,125 @@
     <mergeCell ref="B270:B271"/>
     <mergeCell ref="B250:B256"/>
     <mergeCell ref="B257:B260"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="E68:H68"/>
-    <mergeCell ref="E82:H82"/>
-    <mergeCell ref="E84:H84"/>
-    <mergeCell ref="E90:H90"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="C242:C243"/>
+    <mergeCell ref="B242:B243"/>
+    <mergeCell ref="B244:B247"/>
+    <mergeCell ref="C244:C247"/>
+    <mergeCell ref="B248:B249"/>
+    <mergeCell ref="B229:B230"/>
+    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="B240:B241"/>
+    <mergeCell ref="B231:B239"/>
+    <mergeCell ref="C229:C239"/>
+    <mergeCell ref="B220:B226"/>
+    <mergeCell ref="B227:B228"/>
+    <mergeCell ref="C220:C228"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="B215:B216"/>
+    <mergeCell ref="C210:C216"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="B217:B218"/>
+    <mergeCell ref="B190:B193"/>
+    <mergeCell ref="C184:C193"/>
+    <mergeCell ref="B210:B212"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:C209"/>
+    <mergeCell ref="B205:B207"/>
+    <mergeCell ref="C205:C207"/>
+    <mergeCell ref="C196:C197"/>
+    <mergeCell ref="B196:B197"/>
+    <mergeCell ref="B198:B204"/>
+    <mergeCell ref="C198:C204"/>
+    <mergeCell ref="B194:B195"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="B184:B189"/>
+    <mergeCell ref="B146:B153"/>
+    <mergeCell ref="C141:C153"/>
+    <mergeCell ref="C154:C156"/>
+    <mergeCell ref="B154:B156"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="B133:B135"/>
+    <mergeCell ref="C133:C135"/>
+    <mergeCell ref="B136:B140"/>
+    <mergeCell ref="C136:C140"/>
+    <mergeCell ref="B141:B145"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="C129:C132"/>
+    <mergeCell ref="B177:B180"/>
+    <mergeCell ref="C173:C180"/>
+    <mergeCell ref="B181:B182"/>
+    <mergeCell ref="C181:C182"/>
+    <mergeCell ref="B161:B168"/>
+    <mergeCell ref="C157:C168"/>
+    <mergeCell ref="B169:B172"/>
+    <mergeCell ref="C169:C172"/>
+    <mergeCell ref="B173:B176"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C126:C128"/>
+    <mergeCell ref="B124:B128"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="B107:B113"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="C107:C119"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B73:B77"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C68:C72"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="C59:C63"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B44:B51"/>
+    <mergeCell ref="C44:C51"/>
+    <mergeCell ref="E168:E189"/>
+    <mergeCell ref="E103:E113"/>
+    <mergeCell ref="E150:E157"/>
+    <mergeCell ref="E114:E149"/>
+    <mergeCell ref="F114:F149"/>
+    <mergeCell ref="F158:F162"/>
+    <mergeCell ref="F163:F167"/>
+    <mergeCell ref="E158:E167"/>
+    <mergeCell ref="E101:AA101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9879,53 +9881,53 @@
   <dimension ref="B2:AE113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="17.19921875" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="15.796875" customWidth="1"/>
-    <col min="5" max="5" width="16.796875" customWidth="1"/>
-    <col min="6" max="6" width="18.19921875" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="19.5" customWidth="1"/>
-    <col min="9" max="9" width="18.796875" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="17.19921875" customWidth="1"/>
-    <col min="12" max="12" width="17.796875" customWidth="1"/>
-    <col min="13" max="13" width="16.19921875" customWidth="1"/>
-    <col min="14" max="14" width="16.796875" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" customWidth="1"/>
     <col min="15" max="16" width="24" customWidth="1"/>
-    <col min="17" max="17" width="21.19921875" customWidth="1"/>
-    <col min="18" max="18" width="18.796875" customWidth="1"/>
-    <col min="19" max="19" width="17.19921875" customWidth="1"/>
-    <col min="20" max="20" width="17.796875" customWidth="1"/>
+    <col min="17" max="17" width="31" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" customWidth="1"/>
+    <col min="19" max="19" width="17.1640625" customWidth="1"/>
+    <col min="20" max="20" width="17.83203125" customWidth="1"/>
     <col min="21" max="21" width="20.5" customWidth="1"/>
     <col min="22" max="22" width="18.5" customWidth="1"/>
     <col min="23" max="23" width="17.5" customWidth="1"/>
     <col min="24" max="24" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" ht="16.2" thickBot="1"/>
-    <row r="3" spans="2:31" ht="16.2" thickBot="1">
-      <c r="B3" s="156" t="s">
+    <row r="2" spans="2:31" ht="17" thickBot="1"/>
+    <row r="3" spans="2:31" ht="17" thickBot="1">
+      <c r="B3" s="162" t="s">
         <v>259</v>
       </c>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="157"/>
-      <c r="M3" s="157"/>
-      <c r="N3" s="157"/>
-      <c r="O3" s="158"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="163"/>
+      <c r="K3" s="163"/>
+      <c r="L3" s="163"/>
+      <c r="M3" s="163"/>
+      <c r="N3" s="163"/>
+      <c r="O3" s="164"/>
       <c r="Q3" s="82"/>
       <c r="R3" s="82"/>
       <c r="S3" s="82"/>
@@ -9942,7 +9944,7 @@
       <c r="AD3" s="27"/>
       <c r="AE3" s="27"/>
     </row>
-    <row r="4" spans="2:31" ht="16.2" thickBot="1">
+    <row r="4" spans="2:31" ht="17" thickBot="1">
       <c r="B4" s="67" t="s">
         <v>268</v>
       </c>
@@ -9985,7 +9987,7 @@
       <c r="O4" s="69" t="s">
         <v>287</v>
       </c>
-      <c r="P4" s="162" t="s">
+      <c r="P4" s="110" t="s">
         <v>288</v>
       </c>
       <c r="Q4" s="83" t="s">
@@ -10007,7 +10009,7 @@
       <c r="AE4" s="27"/>
     </row>
     <row r="5" spans="2:31">
-      <c r="B5" s="159" t="s">
+      <c r="B5" s="165" t="s">
         <v>162</v>
       </c>
       <c r="C5" s="97" t="s">
@@ -10046,7 +10048,7 @@
       <c r="AE5" s="27"/>
     </row>
     <row r="6" spans="2:31">
-      <c r="B6" s="160"/>
+      <c r="B6" s="166"/>
       <c r="C6" s="98" t="s">
         <v>167</v>
       </c>
@@ -10083,7 +10085,7 @@
       <c r="AE6" s="27"/>
     </row>
     <row r="7" spans="2:31">
-      <c r="B7" s="160"/>
+      <c r="B7" s="166"/>
       <c r="C7" s="98" t="s">
         <v>168</v>
       </c>
@@ -10120,7 +10122,7 @@
       <c r="AE7" s="27"/>
     </row>
     <row r="8" spans="2:31">
-      <c r="B8" s="160"/>
+      <c r="B8" s="166"/>
       <c r="C8" s="98" t="s">
         <v>169</v>
       </c>
@@ -10157,7 +10159,7 @@
       <c r="AE8" s="27"/>
     </row>
     <row r="9" spans="2:31">
-      <c r="B9" s="160"/>
+      <c r="B9" s="166"/>
       <c r="C9" s="98" t="s">
         <v>170</v>
       </c>
@@ -10194,7 +10196,7 @@
       <c r="AE9" s="27"/>
     </row>
     <row r="10" spans="2:31">
-      <c r="B10" s="160"/>
+      <c r="B10" s="166"/>
       <c r="C10" s="98" t="s">
         <v>171</v>
       </c>
@@ -10231,7 +10233,7 @@
       <c r="AE10" s="27"/>
     </row>
     <row r="11" spans="2:31">
-      <c r="B11" s="160"/>
+      <c r="B11" s="166"/>
       <c r="C11" s="98" t="s">
         <v>172</v>
       </c>
@@ -10268,7 +10270,7 @@
       <c r="AE11" s="27"/>
     </row>
     <row r="12" spans="2:31">
-      <c r="B12" s="160"/>
+      <c r="B12" s="166"/>
       <c r="C12" s="98" t="s">
         <v>173</v>
       </c>
@@ -10305,7 +10307,7 @@
       <c r="AE12" s="27"/>
     </row>
     <row r="13" spans="2:31">
-      <c r="B13" s="160"/>
+      <c r="B13" s="166"/>
       <c r="C13" s="98" t="s">
         <v>174</v>
       </c>
@@ -10342,7 +10344,7 @@
       <c r="AE13" s="27"/>
     </row>
     <row r="14" spans="2:31">
-      <c r="B14" s="160"/>
+      <c r="B14" s="166"/>
       <c r="C14" s="98" t="s">
         <v>175</v>
       </c>
@@ -10378,8 +10380,8 @@
       <c r="AD14" s="27"/>
       <c r="AE14" s="27"/>
     </row>
-    <row r="15" spans="2:31" ht="16.2" thickBot="1">
-      <c r="B15" s="160"/>
+    <row r="15" spans="2:31" ht="17" thickBot="1">
+      <c r="B15" s="166"/>
       <c r="C15" s="103" t="s">
         <v>176</v>
       </c>
@@ -10415,8 +10417,8 @@
       <c r="AD15" s="27"/>
       <c r="AE15" s="27"/>
     </row>
-    <row r="16" spans="2:31" ht="16.05" customHeight="1">
-      <c r="B16" s="159" t="s">
+    <row r="16" spans="2:31" ht="16" customHeight="1">
+      <c r="B16" s="165" t="s">
         <v>261</v>
       </c>
       <c r="C16" s="104" t="s">
@@ -10452,8 +10454,8 @@
       <c r="AD16" s="27"/>
       <c r="AE16" s="27"/>
     </row>
-    <row r="17" spans="2:31">
-      <c r="B17" s="160"/>
+    <row r="17" spans="2:31" ht="17">
+      <c r="B17" s="166"/>
       <c r="C17" s="105" t="s">
         <v>275</v>
       </c>
@@ -10487,8 +10489,8 @@
       <c r="AD17" s="27"/>
       <c r="AE17" s="27"/>
     </row>
-    <row r="18" spans="2:31">
-      <c r="B18" s="160"/>
+    <row r="18" spans="2:31" ht="17">
+      <c r="B18" s="166"/>
       <c r="C18" s="105" t="s">
         <v>276</v>
       </c>
@@ -10522,8 +10524,8 @@
       <c r="AD18" s="27"/>
       <c r="AE18" s="27"/>
     </row>
-    <row r="19" spans="2:31">
-      <c r="B19" s="160"/>
+    <row r="19" spans="2:31" ht="17">
+      <c r="B19" s="166"/>
       <c r="C19" s="105" t="s">
         <v>277</v>
       </c>
@@ -10557,8 +10559,8 @@
       <c r="AD19" s="27"/>
       <c r="AE19" s="27"/>
     </row>
-    <row r="20" spans="2:31" ht="16.2" thickBot="1">
-      <c r="B20" s="160"/>
+    <row r="20" spans="2:31" ht="18" thickBot="1">
+      <c r="B20" s="166"/>
       <c r="C20" s="106" t="s">
         <v>278</v>
       </c>
@@ -10593,7 +10595,7 @@
       <c r="AE20" s="27"/>
     </row>
     <row r="21" spans="2:31">
-      <c r="B21" s="159" t="s">
+      <c r="B21" s="165" t="s">
         <v>260</v>
       </c>
       <c r="C21" s="98" t="s">
@@ -10646,7 +10648,7 @@
       <c r="AE21" s="27"/>
     </row>
     <row r="22" spans="2:31">
-      <c r="B22" s="160"/>
+      <c r="B22" s="166"/>
       <c r="C22" s="98" t="s">
         <v>189</v>
       </c>
@@ -10689,7 +10691,7 @@
       <c r="AE22" s="27"/>
     </row>
     <row r="23" spans="2:31">
-      <c r="B23" s="160"/>
+      <c r="B23" s="166"/>
       <c r="C23" s="98" t="s">
         <v>190</v>
       </c>
@@ -10738,7 +10740,7 @@
       <c r="AE23" s="27"/>
     </row>
     <row r="24" spans="2:31">
-      <c r="B24" s="160"/>
+      <c r="B24" s="166"/>
       <c r="C24" s="98" t="s">
         <v>191</v>
       </c>
@@ -10779,7 +10781,7 @@
       <c r="AE24" s="27"/>
     </row>
     <row r="25" spans="2:31">
-      <c r="B25" s="160"/>
+      <c r="B25" s="166"/>
       <c r="C25" s="98" t="s">
         <v>192</v>
       </c>
@@ -10830,7 +10832,7 @@
       <c r="AE25" s="27"/>
     </row>
     <row r="26" spans="2:31">
-      <c r="B26" s="160"/>
+      <c r="B26" s="166"/>
       <c r="C26" s="98" t="s">
         <v>193</v>
       </c>
@@ -10881,7 +10883,7 @@
       <c r="AE26" s="27"/>
     </row>
     <row r="27" spans="2:31">
-      <c r="B27" s="160"/>
+      <c r="B27" s="166"/>
       <c r="C27" s="98" t="s">
         <v>194</v>
       </c>
@@ -10931,8 +10933,8 @@
       <c r="AD27" s="27"/>
       <c r="AE27" s="27"/>
     </row>
-    <row r="28" spans="2:31" ht="16.2" thickBot="1">
-      <c r="B28" s="161"/>
+    <row r="28" spans="2:31" ht="17" thickBot="1">
+      <c r="B28" s="167"/>
       <c r="C28" s="99" t="s">
         <v>197</v>
       </c>
@@ -10974,12 +10976,12 @@
       <c r="AD28" s="27"/>
       <c r="AE28" s="27"/>
     </row>
-    <row r="29" spans="2:31" ht="15.6" customHeight="1">
-      <c r="B29" s="154" t="s">
+    <row r="29" spans="2:31" ht="15.5" customHeight="1">
+      <c r="B29" s="160" t="s">
         <v>81</v>
       </c>
       <c r="C29" s="108"/>
-      <c r="D29" s="163"/>
+      <c r="D29" s="111"/>
       <c r="E29" s="109"/>
       <c r="F29" s="71"/>
       <c r="G29" s="71"/>
@@ -10990,7 +10992,7 @@
       <c r="L29" s="71"/>
       <c r="M29" s="71"/>
       <c r="N29" s="71"/>
-      <c r="P29" s="164"/>
+      <c r="P29" s="112"/>
       <c r="Q29" s="83"/>
       <c r="R29" s="83"/>
       <c r="S29" s="83"/>
@@ -11007,10 +11009,10 @@
       <c r="AD29" s="27"/>
       <c r="AE29" s="27"/>
     </row>
-    <row r="30" spans="2:31" ht="15.6" customHeight="1">
-      <c r="B30" s="155"/>
+    <row r="30" spans="2:31" ht="15.5" customHeight="1">
+      <c r="B30" s="161"/>
       <c r="C30" s="108"/>
-      <c r="D30" s="163"/>
+      <c r="D30" s="111"/>
       <c r="E30" s="109"/>
       <c r="F30" s="71"/>
       <c r="G30" s="71"/>
@@ -11021,7 +11023,7 @@
       <c r="L30" s="71"/>
       <c r="M30" s="71"/>
       <c r="N30" s="71"/>
-      <c r="P30" s="164"/>
+      <c r="P30" s="112"/>
       <c r="Q30" s="83"/>
       <c r="R30" s="83"/>
       <c r="S30" s="83"/>
@@ -11038,10 +11040,10 @@
       <c r="AD30" s="27"/>
       <c r="AE30" s="27"/>
     </row>
-    <row r="31" spans="2:31" ht="15.6" customHeight="1">
-      <c r="B31" s="155"/>
+    <row r="31" spans="2:31" ht="15.5" customHeight="1">
+      <c r="B31" s="161"/>
       <c r="C31" s="108"/>
-      <c r="D31" s="163"/>
+      <c r="D31" s="111"/>
       <c r="E31" s="109"/>
       <c r="F31" s="71"/>
       <c r="G31" s="71"/>
@@ -11052,7 +11054,7 @@
       <c r="L31" s="71"/>
       <c r="M31" s="71"/>
       <c r="N31" s="71"/>
-      <c r="P31" s="164"/>
+      <c r="P31" s="112"/>
       <c r="Q31" s="83"/>
       <c r="R31" s="83"/>
       <c r="S31" s="83"/>
@@ -11069,10 +11071,10 @@
       <c r="AD31" s="27"/>
       <c r="AE31" s="27"/>
     </row>
-    <row r="32" spans="2:31" ht="15.6" customHeight="1">
-      <c r="B32" s="155"/>
+    <row r="32" spans="2:31" ht="15.5" customHeight="1">
+      <c r="B32" s="161"/>
       <c r="C32" s="108"/>
-      <c r="D32" s="163"/>
+      <c r="D32" s="111"/>
       <c r="E32" s="109"/>
       <c r="F32" s="71"/>
       <c r="G32" s="71"/>
@@ -11083,7 +11085,7 @@
       <c r="L32" s="71"/>
       <c r="M32" s="71"/>
       <c r="N32" s="71"/>
-      <c r="P32" s="164"/>
+      <c r="P32" s="112"/>
       <c r="Q32" s="83"/>
       <c r="R32" s="83"/>
       <c r="S32" s="83"/>
@@ -11100,10 +11102,10 @@
       <c r="AD32" s="27"/>
       <c r="AE32" s="27"/>
     </row>
-    <row r="33" spans="2:31" ht="15.6" customHeight="1">
-      <c r="B33" s="155"/>
+    <row r="33" spans="2:31" ht="15.5" customHeight="1">
+      <c r="B33" s="161"/>
       <c r="C33" s="108"/>
-      <c r="D33" s="163"/>
+      <c r="D33" s="111"/>
       <c r="E33" s="109"/>
       <c r="F33" s="71"/>
       <c r="G33" s="71"/>
@@ -11114,7 +11116,7 @@
       <c r="L33" s="71"/>
       <c r="M33" s="71"/>
       <c r="N33" s="71"/>
-      <c r="P33" s="164"/>
+      <c r="P33" s="112"/>
       <c r="Q33" s="83"/>
       <c r="R33" s="83"/>
       <c r="S33" s="83"/>
@@ -11131,10 +11133,10 @@
       <c r="AD33" s="27"/>
       <c r="AE33" s="27"/>
     </row>
-    <row r="34" spans="2:31" ht="15.6" customHeight="1">
-      <c r="B34" s="155"/>
+    <row r="34" spans="2:31" ht="15.5" customHeight="1">
+      <c r="B34" s="161"/>
       <c r="C34" s="108"/>
-      <c r="D34" s="163"/>
+      <c r="D34" s="111"/>
       <c r="E34" s="109"/>
       <c r="F34" s="71"/>
       <c r="G34" s="71"/>
@@ -11145,7 +11147,7 @@
       <c r="L34" s="71"/>
       <c r="M34" s="71"/>
       <c r="N34" s="71"/>
-      <c r="P34" s="164"/>
+      <c r="P34" s="112"/>
       <c r="Q34" s="83"/>
       <c r="R34" s="83"/>
       <c r="S34" s="83"/>
@@ -11162,10 +11164,10 @@
       <c r="AD34" s="27"/>
       <c r="AE34" s="27"/>
     </row>
-    <row r="35" spans="2:31" ht="15.6" customHeight="1">
-      <c r="B35" s="155"/>
+    <row r="35" spans="2:31" ht="15.5" customHeight="1">
+      <c r="B35" s="161"/>
       <c r="C35" s="108"/>
-      <c r="D35" s="163"/>
+      <c r="D35" s="111"/>
       <c r="E35" s="109"/>
       <c r="F35" s="71"/>
       <c r="G35" s="71"/>
@@ -11176,7 +11178,7 @@
       <c r="L35" s="71"/>
       <c r="M35" s="71"/>
       <c r="N35" s="71"/>
-      <c r="P35" s="164"/>
+      <c r="P35" s="112"/>
       <c r="Q35" s="83"/>
       <c r="R35" s="83"/>
       <c r="S35" s="83"/>
@@ -11193,10 +11195,10 @@
       <c r="AD35" s="27"/>
       <c r="AE35" s="27"/>
     </row>
-    <row r="36" spans="2:31" ht="15.6" customHeight="1">
-      <c r="B36" s="155"/>
+    <row r="36" spans="2:31" ht="15.5" customHeight="1">
+      <c r="B36" s="161"/>
       <c r="C36" s="108"/>
-      <c r="D36" s="163"/>
+      <c r="D36" s="111"/>
       <c r="E36" s="109"/>
       <c r="F36" s="71"/>
       <c r="G36" s="71"/>
@@ -11207,7 +11209,7 @@
       <c r="L36" s="71"/>
       <c r="M36" s="71"/>
       <c r="N36" s="71"/>
-      <c r="P36" s="164"/>
+      <c r="P36" s="112"/>
       <c r="Q36" s="83"/>
       <c r="R36" s="83"/>
       <c r="S36" s="83"/>
@@ -11224,10 +11226,10 @@
       <c r="AD36" s="27"/>
       <c r="AE36" s="27"/>
     </row>
-    <row r="37" spans="2:31" ht="16.05" customHeight="1" thickBot="1">
-      <c r="B37" s="155"/>
+    <row r="37" spans="2:31" ht="16" customHeight="1" thickBot="1">
+      <c r="B37" s="161"/>
       <c r="C37" s="108"/>
-      <c r="D37" s="163"/>
+      <c r="D37" s="111"/>
       <c r="E37" s="109"/>
       <c r="F37" s="71"/>
       <c r="G37" s="71"/>
@@ -11238,7 +11240,7 @@
       <c r="L37" s="71"/>
       <c r="M37" s="71"/>
       <c r="N37" s="71"/>
-      <c r="P37" s="164"/>
+      <c r="P37" s="112"/>
       <c r="Q37" s="83"/>
       <c r="R37" s="83"/>
       <c r="S37" s="83"/>
@@ -11255,10 +11257,10 @@
       <c r="AD37" s="27"/>
       <c r="AE37" s="27"/>
     </row>
-    <row r="38" spans="2:31" ht="16.2" thickBot="1">
-      <c r="B38" s="155"/>
+    <row r="38" spans="2:31" ht="17" thickBot="1">
+      <c r="B38" s="161"/>
       <c r="C38" s="107"/>
-      <c r="D38" s="163"/>
+      <c r="D38" s="111"/>
       <c r="E38" s="109"/>
       <c r="F38" s="71"/>
       <c r="G38" s="71"/>
@@ -11269,7 +11271,7 @@
       <c r="L38" s="71"/>
       <c r="M38" s="71"/>
       <c r="N38" s="71"/>
-      <c r="P38" s="164"/>
+      <c r="P38" s="112"/>
       <c r="Q38" s="83"/>
       <c r="R38" s="83"/>
       <c r="S38" s="83"/>
@@ -11286,8 +11288,8 @@
       <c r="AD38" s="27"/>
       <c r="AE38" s="27"/>
     </row>
-    <row r="39" spans="2:31">
-      <c r="B39" s="151" t="s">
+    <row r="39" spans="2:31" ht="17">
+      <c r="B39" s="157" t="s">
         <v>105</v>
       </c>
       <c r="C39" s="100" t="s">
@@ -11304,7 +11306,7 @@
       <c r="L39" s="90"/>
       <c r="M39" s="90"/>
       <c r="N39" s="90"/>
-      <c r="Q39" s="165" t="s">
+      <c r="Q39" s="113" t="s">
         <v>284</v>
       </c>
       <c r="R39" s="83"/>
@@ -11322,8 +11324,8 @@
       <c r="AD39" s="27"/>
       <c r="AE39" s="27"/>
     </row>
-    <row r="40" spans="2:31">
-      <c r="B40" s="152"/>
+    <row r="40" spans="2:31" ht="17">
+      <c r="B40" s="158"/>
       <c r="C40" s="101" t="s">
         <v>201</v>
       </c>
@@ -11338,7 +11340,7 @@
       <c r="L40" s="85"/>
       <c r="M40" s="85"/>
       <c r="N40" s="85"/>
-      <c r="Q40" s="166" t="s">
+      <c r="Q40" s="114" t="s">
         <v>286</v>
       </c>
       <c r="R40" s="83"/>
@@ -11356,8 +11358,8 @@
       <c r="AD40" s="27"/>
       <c r="AE40" s="27"/>
     </row>
-    <row r="41" spans="2:31" ht="16.2" thickBot="1">
-      <c r="B41" s="153"/>
+    <row r="41" spans="2:31" ht="18" thickBot="1">
+      <c r="B41" s="159"/>
       <c r="C41" s="102" t="s">
         <v>202</v>
       </c>
@@ -11372,7 +11374,7 @@
       <c r="L41" s="92"/>
       <c r="M41" s="92"/>
       <c r="N41" s="92"/>
-      <c r="Q41" s="167" t="s">
+      <c r="Q41" s="115" t="s">
         <v>285</v>
       </c>
       <c r="R41" s="83"/>
@@ -11390,7 +11392,7 @@
       <c r="AD41" s="27"/>
       <c r="AE41" s="27"/>
     </row>
-    <row r="42" spans="2:31" ht="16.05" customHeight="1">
+    <row r="42" spans="2:31" ht="16" customHeight="1">
       <c r="B42" s="84"/>
       <c r="C42" s="84"/>
       <c r="D42" s="83"/>
@@ -11550,7 +11552,7 @@
       <c r="AD46" s="27"/>
       <c r="AE46" s="27"/>
     </row>
-    <row r="47" spans="2:31" ht="16.05" customHeight="1">
+    <row r="47" spans="2:31" ht="16" customHeight="1">
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
       <c r="D47" s="27"/>

</xml_diff>

<commit_message>
Finalized Master Template and uploaded SUBMISSION
</commit_message>
<xml_diff>
--- a/in-progress/Koerner_2005_Polymer/Koerner_2005_Polymer_Tidy_Table.xlsx
+++ b/in-progress/Koerner_2005_Polymer/Koerner_2005_Polymer_Tidy_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/in-progress/Koerner_2005_Polymer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C77976-73C2-E848-9757-E7EA80941A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42084AA8-4DDF-8745-A358-ABC0B65DEBCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7980" yWindow="460" windowWidth="20780" windowHeight="17540" xr2:uid="{AA27EEF6-2707-3642-A9D6-F1434A24BCB7}"/>
   </bookViews>
@@ -860,7 +860,7 @@
   <dimension ref="A1:AD105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,7 +1427,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="30">
-        <v>0.1400732622863767</v>
+        <v>0</v>
       </c>
       <c r="C18" s="22">
         <v>14.03061224</v>
@@ -1759,7 +1759,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="1">
-        <v>-3.9049385988164403E-2</v>
+        <v>0</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>

</xml_diff>